<commit_message>
all hw1 done, except for big doubts
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week3/hw1.xlsx
+++ b/PM2/econ/week3/hw1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710D5FC0-984C-4ADF-AE43-F3ED26692809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCC7F1E-0DAF-4E58-B5B2-DBA4C215FF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="28" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="20" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
   </bookViews>
   <sheets>
     <sheet name="ex1" sheetId="1" r:id="rId1"/>
@@ -24,22 +24,22 @@
     <sheet name="ex9" sheetId="9" r:id="rId9"/>
     <sheet name="ex10" sheetId="10" r:id="rId10"/>
     <sheet name="ex11" sheetId="11" r:id="rId11"/>
-    <sheet name="ex12" sheetId="12" r:id="rId12"/>
+    <sheet name="ex12b" sheetId="12" r:id="rId12"/>
     <sheet name="ex13" sheetId="13" r:id="rId13"/>
     <sheet name="ex14" sheetId="14" r:id="rId14"/>
     <sheet name="ex15" sheetId="15" r:id="rId15"/>
     <sheet name="ex16" sheetId="16" r:id="rId16"/>
     <sheet name="ex17" sheetId="17" r:id="rId17"/>
     <sheet name="ex18" sheetId="18" r:id="rId18"/>
-    <sheet name="ex19" sheetId="19" r:id="rId19"/>
+    <sheet name="ex19b" sheetId="19" r:id="rId19"/>
     <sheet name="ex20" sheetId="20" r:id="rId20"/>
-    <sheet name="ex21b" sheetId="21" r:id="rId21"/>
+    <sheet name="ex21" sheetId="21" r:id="rId21"/>
     <sheet name="ex22" sheetId="22" r:id="rId22"/>
     <sheet name="ex23" sheetId="23" r:id="rId23"/>
     <sheet name="ex24" sheetId="24" r:id="rId24"/>
     <sheet name="ex25" sheetId="25" r:id="rId25"/>
     <sheet name="ex26b" sheetId="26" r:id="rId26"/>
-    <sheet name="ex27b" sheetId="27" r:id="rId27"/>
+    <sheet name="ex27" sheetId="27" r:id="rId27"/>
     <sheet name="ex28" sheetId="28" r:id="rId28"/>
     <sheet name="ex29" sheetId="29" r:id="rId29"/>
     <sheet name="ex30" sheetId="30" r:id="rId30"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="79">
   <si>
     <t>Flujos</t>
   </si>
@@ -190,9 +190,6 @@
     <t>hoy</t>
   </si>
   <si>
-    <t>sacar</t>
-  </si>
-  <si>
     <t>plazo</t>
   </si>
   <si>
@@ -279,14 +276,41 @@
   <si>
     <t>deposito</t>
   </si>
+  <si>
+    <t>supongo que es me prestan 2000 a pagar en 2 años, cuanto sera la mensualidad?</t>
+  </si>
+  <si>
+    <t>mensualidad</t>
+  </si>
+  <si>
+    <t>tasa real a largo plazo?</t>
+  </si>
+  <si>
+    <t>ahorro/mes</t>
+  </si>
+  <si>
+    <t>accum</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>suma de VP de 11 a inf debe ahorrarse del 0 al 10</t>
+  </si>
+  <si>
+    <t>como es VP hasta el año 10, todo esto lo llevo VF al 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -512,7 +536,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -521,30 +545,30 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -564,6 +588,1152 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-419"/>
+              <a:t>Suma</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-419" baseline="0"/>
+              <a:t> acumulada de VP al año 10</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ex21'!$N$12:$DN$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="105"/>
+                <c:pt idx="0">
+                  <c:v>18181.81818181818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34710.74380165289</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49737.03981968444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63397.308926985846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75815.735388168949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87105.213989244497</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97368.376353858621</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106698.52395805328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>115180.47632550297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>122891.3421140936</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>129901.22010372144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>136273.83645792858</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>142067.12405266234</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>147333.74913878393</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>152121.5901261672</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>156474.17284197017</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160431.06621997288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>164028.24201815715</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>167298.40183468829</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>170271.27439517117</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>172973.88581379197</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>175430.80528526541</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>177664.36844115035</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>179694.88040104575</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>181540.80036458705</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>183218.90942235186</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>184744.46311122895</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>186131.3301011172</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>187392.1182737429</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>188538.28933976626</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>189580.26303615113</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>190527.51185104647</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>191388.64713731495</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>192171.49739755903</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>192883.17945232638</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>193530.16313847853</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>194118.33012588957</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>194653.02738717233</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195139.11580652031</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>195581.0143695639</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>195982.74033596716</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>196347.94575997014</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>196679.95069088193</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>196981.77335534719</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>197256.15759577017</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>197505.59781433651</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>197732.3616493968</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>197938.5105903607</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>198125.91871850973</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>198296.28974409975</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>198451.17249463612</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>198591.97499512375</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>198719.97726829431</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>198836.34297117664</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>198942.12997379692</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>199038.299976179</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>199125.7272510718</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>199205.20659188344</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>199277.46053807583</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>199343.14594370528</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>199402.85994882297</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>199457.14540802088</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>199506.49582547351</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>199551.35984133955</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>199592.14531030867</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>199629.22300937149</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>199662.93000851953</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>199693.57273501775</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>199721.42975910704</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>199746.75432646094</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>199769.77666041904</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>199790.70605492638</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>199809.73277720579</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>199827.02979745981</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>199842.7543613271</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>199857.04941938826</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>199870.0449267166</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>199881.85902428781</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>199892.59911298892</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>199902.36282998993</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>199911.23893635446</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>199919.30812395859</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>199926.64374905324</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>199933.31249913931</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>199939.37499921754</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>199944.88636292503</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>199949.89669356821</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>199954.45153960746</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>199958.59230873405</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>199962.35664430368</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>199965.77876754879</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>199968.88978868071</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>199971.71798970972</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>199974.28908155428</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>199976.62643777661</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>199978.75130706964</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>199980.68300642693</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>199982.43909675174</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>199984.03554250157</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>199985.4868568196</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>199986.80623347234</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>199988.00566679303</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>199989.09606072094</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>199990.08732792811</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>199990.98847993463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BE64-4995-8F19-9C160EADDD20}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1857564512"/>
+        <c:axId val="1857565344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1857564512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1857565344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1857565344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1857564512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1346,7 +2516,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>373446</xdr:colOff>
+      <xdr:colOff>196084</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>169653</xdr:rowOff>
     </xdr:to>
@@ -1373,6 +2543,86 @@
         <a:xfrm>
           <a:off x="154371" y="82440"/>
           <a:ext cx="6328213" cy="1039713"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>604632</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>135836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>273328</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>21536</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C84024-0590-BC9D-7C1C-ABD2273CDDED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>530085</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504498</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>37141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A55CAC3-E288-7F31-DD2C-E249E7DFC468}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="530085" y="3752022"/>
+          <a:ext cx="2600000" cy="1047619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1684,7 +2934,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>504826</xdr:colOff>
+      <xdr:colOff>307757</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>30508</xdr:rowOff>
     </xdr:to>
@@ -2934,7 +4184,7 @@
         <v>8333.3333333333339</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="D10:G10" si="0">E8/((1+E9)^(E7))</f>
+        <f t="shared" ref="E10:G10" si="0">E8/((1+E9)^(E7))</f>
         <v>6944.4444444444443</v>
       </c>
       <c r="F10">
@@ -2996,20 +4246,20 @@
       <c r="B9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="23">
         <v>0.15</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <f>(D11/D10)-1</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="23">
         <v>0.15</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="23">
         <v>0.35</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="24">
         <v>0.25</v>
       </c>
     </row>
@@ -3017,43 +4267,43 @@
       <c r="B10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="25">
         <v>0.1</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="25">
         <v>0.15</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="30">
         <f>((1+E11)/(1+E9))-1</f>
         <v>8.6956521739130599E-2</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25">
         <v>0.15</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="32">
         <f>((1+G11)/(1+G9))-1</f>
         <v>8.0000000000000071E-2</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="28">
         <f>(1+C10)*(1+C9)-1</f>
         <v>0.2649999999999999</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="26">
         <v>0.25</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="26">
         <v>0.25</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="31">
         <f>(1+F10)*(1+F9)-1</f>
         <v>0.55249999999999999</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="27">
         <v>0.35</v>
       </c>
     </row>
@@ -3094,10 +4344,10 @@
       <c r="C7" s="1">
         <v>0.05</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="33">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="33">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
@@ -3108,7 +4358,7 @@
       <c r="C8">
         <v>105</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9">
@@ -3131,7 +4381,7 @@
   <dimension ref="C7:F9"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,14 +4398,14 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="35"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="1">
         <v>0.05</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="33">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="33">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
@@ -3163,15 +4413,15 @@
       <c r="C9">
         <v>2.8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f>C9*(1+D8)</f>
         <v>2.94</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f>C9*(1+D8)*(1+E8)</f>
         <v>3.1311</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <f>C9*(1+D8)*(1+E8)*(1+F8)</f>
         <v>3.2719994999999997</v>
       </c>
@@ -3256,7 +4506,7 @@
       <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="34">
         <f>((1+D7)/(1+D6))-1</f>
         <v>8.6956521739130599E-2</v>
       </c>
@@ -3363,13 +4613,13 @@
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="35">
         <v>0</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="35">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="35">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F11" s="1">
@@ -3582,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="9">
-        <f t="shared" ref="L16:O16" si="0">E16/((1+$C$16)^(L15-$K$15))</f>
+        <f t="shared" ref="L16:N16" si="0">E16/((1+$C$16)^(L15-$K$15))</f>
         <v>47.61904761904762</v>
       </c>
       <c r="M16" s="9">
@@ -3698,7 +4948,7 @@
         <v>102.45201830476057</v>
       </c>
       <c r="P18" s="9">
-        <f t="shared" ref="P17:P24" si="3">SUM(K18:O18)</f>
+        <f t="shared" ref="P18:P24" si="3">SUM(K18:O18)</f>
         <v>303.80438494638338</v>
       </c>
     </row>
@@ -3986,7 +5236,7 @@
         <v>230.76923076923077</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" ref="L24:O24" si="9">F24/((1+$C$24)^(M15-$K$15))</f>
+        <f t="shared" ref="M24:O24" si="9">F24/((1+$C$24)^(M15-$K$15))</f>
         <v>295.85798816568047</v>
       </c>
       <c r="N24" s="9">
@@ -4010,10 +5260,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3C1205-B505-47CC-9F42-6948E774DB05}">
-  <dimension ref="B6:AR9"/>
+  <dimension ref="B6:AR12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4311,6 +5561,11 @@
       <c r="C9" s="2">
         <f>AR8/((1+B8)^(40))</f>
         <v>50737.65494327456</v>
+      </c>
+    </row>
+    <row r="12" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4321,20 +5576,23 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4899B06-D786-4CEC-8B8A-040F849CA034}">
-  <dimension ref="B7:S10"/>
+  <dimension ref="A7:DN19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:118" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:118" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>0.1</v>
       </c>
@@ -4368,7 +5626,7 @@
       <c r="L8">
         <v>9</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="18">
         <v>10</v>
       </c>
       <c r="N8">
@@ -4386,13 +5644,354 @@
       <c r="R8">
         <v>15</v>
       </c>
-      <c r="S8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <v>16</v>
+      </c>
+      <c r="T8">
+        <v>17</v>
+      </c>
+      <c r="U8">
+        <v>18</v>
+      </c>
+      <c r="V8">
+        <v>19</v>
+      </c>
+      <c r="W8">
+        <v>20</v>
+      </c>
+      <c r="X8">
+        <v>21</v>
+      </c>
+      <c r="Y8">
+        <v>22</v>
+      </c>
+      <c r="Z8">
+        <v>23</v>
+      </c>
+      <c r="AA8">
+        <v>24</v>
+      </c>
+      <c r="AB8">
+        <v>25</v>
+      </c>
+      <c r="AC8">
+        <v>26</v>
+      </c>
+      <c r="AD8">
+        <v>27</v>
+      </c>
+      <c r="AE8">
+        <v>28</v>
+      </c>
+      <c r="AF8">
+        <v>29</v>
+      </c>
+      <c r="AG8">
+        <v>30</v>
+      </c>
+      <c r="AH8">
+        <v>31</v>
+      </c>
+      <c r="AI8">
+        <v>32</v>
+      </c>
+      <c r="AJ8">
+        <v>33</v>
+      </c>
+      <c r="AK8">
+        <v>34</v>
+      </c>
+      <c r="AL8">
+        <v>35</v>
+      </c>
+      <c r="AM8">
+        <v>36</v>
+      </c>
+      <c r="AN8">
+        <v>37</v>
+      </c>
+      <c r="AO8">
+        <v>38</v>
+      </c>
+      <c r="AP8">
+        <v>39</v>
+      </c>
+      <c r="AQ8">
+        <v>40</v>
+      </c>
+      <c r="AR8">
+        <v>41</v>
+      </c>
+      <c r="AS8">
+        <v>42</v>
+      </c>
+      <c r="AT8">
+        <v>43</v>
+      </c>
+      <c r="AU8">
+        <v>44</v>
+      </c>
+      <c r="AV8">
+        <v>45</v>
+      </c>
+      <c r="AW8">
+        <v>46</v>
+      </c>
+      <c r="AX8">
+        <v>47</v>
+      </c>
+      <c r="AY8">
+        <v>48</v>
+      </c>
+      <c r="AZ8">
+        <v>49</v>
+      </c>
+      <c r="BA8">
+        <v>50</v>
+      </c>
+      <c r="BB8">
+        <v>51</v>
+      </c>
+      <c r="BC8">
+        <v>52</v>
+      </c>
+      <c r="BD8">
+        <v>53</v>
+      </c>
+      <c r="BE8">
+        <v>54</v>
+      </c>
+      <c r="BF8">
+        <v>55</v>
+      </c>
+      <c r="BG8">
+        <v>56</v>
+      </c>
+      <c r="BH8">
+        <v>57</v>
+      </c>
+      <c r="BI8">
+        <v>58</v>
+      </c>
+      <c r="BJ8">
+        <v>59</v>
+      </c>
+      <c r="BK8">
+        <v>60</v>
+      </c>
+      <c r="BL8">
+        <v>61</v>
+      </c>
+      <c r="BM8">
+        <v>62</v>
+      </c>
+      <c r="BN8">
+        <v>63</v>
+      </c>
+      <c r="BO8">
+        <v>64</v>
+      </c>
+      <c r="BP8">
+        <v>65</v>
+      </c>
+      <c r="BQ8">
+        <v>66</v>
+      </c>
+      <c r="BR8">
+        <v>67</v>
+      </c>
+      <c r="BS8">
+        <v>68</v>
+      </c>
+      <c r="BT8">
+        <v>69</v>
+      </c>
+      <c r="BU8">
+        <v>70</v>
+      </c>
+      <c r="BV8">
+        <v>71</v>
+      </c>
+      <c r="BW8">
+        <v>72</v>
+      </c>
+      <c r="BX8">
+        <v>73</v>
+      </c>
+      <c r="BY8">
+        <v>74</v>
+      </c>
+      <c r="BZ8">
+        <v>75</v>
+      </c>
+      <c r="CA8">
+        <v>76</v>
+      </c>
+      <c r="CB8">
+        <v>77</v>
+      </c>
+      <c r="CC8">
+        <v>78</v>
+      </c>
+      <c r="CD8">
+        <v>79</v>
+      </c>
+      <c r="CE8">
+        <v>80</v>
+      </c>
+      <c r="CF8">
+        <v>81</v>
+      </c>
+      <c r="CG8">
+        <v>82</v>
+      </c>
+      <c r="CH8">
+        <v>83</v>
+      </c>
+      <c r="CI8">
+        <v>84</v>
+      </c>
+      <c r="CJ8">
+        <v>85</v>
+      </c>
+      <c r="CK8">
+        <v>86</v>
+      </c>
+      <c r="CL8">
+        <v>87</v>
+      </c>
+      <c r="CM8">
+        <v>88</v>
+      </c>
+      <c r="CN8">
+        <v>89</v>
+      </c>
+      <c r="CO8">
+        <v>90</v>
+      </c>
+      <c r="CP8">
+        <v>91</v>
+      </c>
+      <c r="CQ8">
+        <v>92</v>
+      </c>
+      <c r="CR8">
+        <v>93</v>
+      </c>
+      <c r="CS8">
+        <v>94</v>
+      </c>
+      <c r="CT8">
+        <v>95</v>
+      </c>
+      <c r="CU8">
+        <v>96</v>
+      </c>
+      <c r="CV8">
+        <v>97</v>
+      </c>
+      <c r="CW8">
+        <v>98</v>
+      </c>
+      <c r="CX8">
+        <v>99</v>
+      </c>
+      <c r="CY8">
+        <v>100</v>
+      </c>
+      <c r="CZ8">
+        <v>101</v>
+      </c>
+      <c r="DA8">
+        <v>102</v>
+      </c>
+      <c r="DB8">
+        <v>103</v>
+      </c>
+      <c r="DC8">
+        <v>104</v>
+      </c>
+      <c r="DD8">
+        <v>105</v>
+      </c>
+      <c r="DE8">
+        <v>106</v>
+      </c>
+      <c r="DF8">
+        <v>107</v>
+      </c>
+      <c r="DG8">
+        <v>108</v>
+      </c>
+      <c r="DH8">
+        <v>109</v>
+      </c>
+      <c r="DI8">
+        <v>110</v>
+      </c>
+      <c r="DJ8">
+        <v>111</v>
+      </c>
+      <c r="DK8">
+        <v>112</v>
+      </c>
+      <c r="DL8">
+        <v>113</v>
+      </c>
+      <c r="DM8">
+        <v>114</v>
+      </c>
+      <c r="DN8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:118" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$B$14</f>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" ref="D9:M9" si="0">$B$14</f>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
+      </c>
+      <c r="M9" s="38">
+        <f t="shared" si="0"/>
+        <v>10792.142736644701</v>
       </c>
       <c r="N9">
         <v>20000</v>
@@ -4409,34 +6008,1353 @@
       <c r="R9">
         <v>20000</v>
       </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <v>20000</v>
+      </c>
+      <c r="T9">
+        <v>20000</v>
+      </c>
+      <c r="U9">
+        <v>20000</v>
+      </c>
+      <c r="V9">
+        <v>20000</v>
+      </c>
+      <c r="W9">
+        <v>20000</v>
+      </c>
+      <c r="X9">
+        <v>20000</v>
+      </c>
+      <c r="Y9">
+        <v>20000</v>
+      </c>
+      <c r="Z9">
+        <v>20000</v>
+      </c>
+      <c r="AA9">
+        <v>20000</v>
+      </c>
+      <c r="AB9">
+        <v>20000</v>
+      </c>
+      <c r="AC9">
+        <v>20000</v>
+      </c>
+      <c r="AD9">
+        <v>20000</v>
+      </c>
+      <c r="AE9">
+        <v>20000</v>
+      </c>
+      <c r="AF9">
+        <v>20000</v>
+      </c>
+      <c r="AG9">
+        <v>20000</v>
+      </c>
+      <c r="AH9">
+        <v>20000</v>
+      </c>
+      <c r="AI9">
+        <v>20000</v>
+      </c>
+      <c r="AJ9">
+        <v>20000</v>
+      </c>
+      <c r="AK9">
+        <v>20000</v>
+      </c>
+      <c r="AL9">
+        <v>20000</v>
+      </c>
+      <c r="AM9">
+        <v>20000</v>
+      </c>
+      <c r="AN9">
+        <v>20000</v>
+      </c>
+      <c r="AO9">
+        <v>20000</v>
+      </c>
+      <c r="AP9">
+        <v>20000</v>
+      </c>
+      <c r="AQ9">
+        <v>20000</v>
+      </c>
+      <c r="AR9">
+        <v>20000</v>
+      </c>
+      <c r="AS9">
+        <v>20000</v>
+      </c>
+      <c r="AT9">
+        <v>20000</v>
+      </c>
+      <c r="AU9">
+        <v>20000</v>
+      </c>
+      <c r="AV9">
+        <v>20000</v>
+      </c>
+      <c r="AW9">
+        <v>20000</v>
+      </c>
+      <c r="AX9">
+        <v>20000</v>
+      </c>
+      <c r="AY9">
+        <v>20000</v>
+      </c>
+      <c r="AZ9">
+        <v>20000</v>
+      </c>
+      <c r="BA9">
+        <v>20000</v>
+      </c>
+      <c r="BB9">
+        <v>20000</v>
+      </c>
+      <c r="BC9">
+        <v>20000</v>
+      </c>
+      <c r="BD9">
+        <v>20000</v>
+      </c>
+      <c r="BE9">
+        <v>20000</v>
+      </c>
+      <c r="BF9">
+        <v>20000</v>
+      </c>
+      <c r="BG9">
+        <v>20000</v>
+      </c>
+      <c r="BH9">
+        <v>20000</v>
+      </c>
+      <c r="BI9">
+        <v>20000</v>
+      </c>
+      <c r="BJ9">
+        <v>20000</v>
+      </c>
+      <c r="BK9">
+        <v>20000</v>
+      </c>
+      <c r="BL9">
+        <v>20000</v>
+      </c>
+      <c r="BM9">
+        <v>20000</v>
+      </c>
+      <c r="BN9">
+        <v>20000</v>
+      </c>
+      <c r="BO9">
+        <v>20000</v>
+      </c>
+      <c r="BP9">
+        <v>20000</v>
+      </c>
+      <c r="BQ9">
+        <v>20000</v>
+      </c>
+      <c r="BR9">
+        <v>20000</v>
+      </c>
+      <c r="BS9">
+        <v>20000</v>
+      </c>
+      <c r="BT9">
+        <v>20000</v>
+      </c>
+      <c r="BU9">
+        <v>20000</v>
+      </c>
+      <c r="BV9">
+        <v>20000</v>
+      </c>
+      <c r="BW9">
+        <v>20000</v>
+      </c>
+      <c r="BX9">
+        <v>20000</v>
+      </c>
+      <c r="BY9">
+        <v>20000</v>
+      </c>
+      <c r="BZ9">
+        <v>20000</v>
+      </c>
+      <c r="CA9">
+        <v>20000</v>
+      </c>
+      <c r="CB9">
+        <v>20000</v>
+      </c>
+      <c r="CC9">
+        <v>20000</v>
+      </c>
+      <c r="CD9">
+        <v>20000</v>
+      </c>
+      <c r="CE9">
+        <v>20000</v>
+      </c>
+      <c r="CF9">
+        <v>20000</v>
+      </c>
+      <c r="CG9">
+        <v>20000</v>
+      </c>
+      <c r="CH9">
+        <v>20000</v>
+      </c>
+      <c r="CI9">
+        <v>20000</v>
+      </c>
+      <c r="CJ9">
+        <v>20000</v>
+      </c>
+      <c r="CK9">
+        <v>20000</v>
+      </c>
+      <c r="CL9">
+        <v>20000</v>
+      </c>
+      <c r="CM9">
+        <v>20000</v>
+      </c>
+      <c r="CN9">
+        <v>20000</v>
+      </c>
+      <c r="CO9">
+        <v>20000</v>
+      </c>
+      <c r="CP9">
+        <v>20000</v>
+      </c>
+      <c r="CQ9">
+        <v>20000</v>
+      </c>
+      <c r="CR9">
+        <v>20000</v>
+      </c>
+      <c r="CS9">
+        <v>20000</v>
+      </c>
+      <c r="CT9">
+        <v>20000</v>
+      </c>
+      <c r="CU9">
+        <v>20000</v>
+      </c>
+      <c r="CV9">
+        <v>20000</v>
+      </c>
+      <c r="CW9">
+        <v>20000</v>
+      </c>
+      <c r="CX9">
+        <v>20000</v>
+      </c>
+      <c r="CY9">
+        <v>20000</v>
+      </c>
+      <c r="CZ9">
+        <v>20000</v>
+      </c>
+      <c r="DA9">
+        <v>20000</v>
+      </c>
+      <c r="DB9">
+        <v>20000</v>
+      </c>
+      <c r="DC9">
+        <v>20000</v>
+      </c>
+      <c r="DD9">
+        <v>20000</v>
+      </c>
+      <c r="DE9">
+        <v>20000</v>
+      </c>
+      <c r="DF9">
+        <v>20000</v>
+      </c>
+      <c r="DG9">
+        <v>20000</v>
+      </c>
+      <c r="DH9">
+        <v>20000</v>
+      </c>
+      <c r="DI9">
+        <v>20000</v>
+      </c>
+      <c r="DJ9">
+        <v>20000</v>
+      </c>
+      <c r="DK9">
+        <v>20000</v>
+      </c>
+      <c r="DL9">
+        <v>20000</v>
+      </c>
+      <c r="DM9">
+        <v>20000</v>
+      </c>
+      <c r="DN9">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:118" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <f>C9*(1+$B$8)^($M$8-C8)</f>
+        <v>27992.038851495192</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:M10" si="1">D9*(1+$B$8)^($M$8-D8)</f>
+        <v>25447.308046813807</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>23133.91640619437</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>21030.833096540337</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>19118.93917867303</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>17380.853798793662</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>15800.77618072151</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>14364.341982474101</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>13058.49271134009</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>11871.357010309172</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="1"/>
+        <v>10792.142736644701</v>
       </c>
       <c r="N10">
-        <f>N9/((1+$B$8)^($R$8-N8))</f>
+        <f>N9/((1+$B$8)^(N8-$M$8))</f>
+        <v>18181.81818181818</v>
+      </c>
+      <c r="O10">
+        <f>O9/((1+$B$8)^(O8-$M$8))</f>
+        <v>16528.925619834707</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="O10:Q10" si="2">P9/((1+$B$8)^(P8-$M$8))</f>
+        <v>15026.296018031551</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
         <v>13660.26910730141</v>
       </c>
-      <c r="O10">
-        <f t="shared" ref="O10:R10" si="0">O9/((1+$B$8)^($R$8-O8))</f>
-        <v>15026.296018031551</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>16528.925619834707</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="0"/>
+      <c r="R10">
+        <f>R9/((1+$B$8)^(R8-$M$8))</f>
+        <v>12418.426461183099</v>
+      </c>
+      <c r="S10">
+        <f>S9/((1+$B$8)^(S8-$M$8))</f>
+        <v>11289.478601075543</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ref="T10" si="3">T9/((1+$B$8)^(T8-$M$8))</f>
+        <v>10263.162364614129</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10" si="4">U9/((1+$B$8)^(U8-$M$8))</f>
+        <v>9330.1476041946626</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ref="V10" si="5">V9/((1+$B$8)^(V8-$M$8))</f>
+        <v>8481.9523674496941</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ref="W10" si="6">W9/((1+$B$8)^(W8-$M$8))</f>
+        <v>7710.8657885906296</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ref="X10" si="7">X9/((1+$B$8)^(X8-$M$8))</f>
+        <v>7009.8779896278438</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" ref="Y10" si="8">Y9/((1+$B$8)^(Y8-$M$8))</f>
+        <v>6372.6163542071308</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" ref="Z10" si="9">Z9/((1+$B$8)^(Z8-$M$8))</f>
+        <v>5793.2875947337552</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" ref="AA10" si="10">AA9/((1+$B$8)^(AA8-$M$8))</f>
+        <v>5266.6250861215949</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" ref="AB10" si="11">AB9/((1+$B$8)^(AB8-$M$8))</f>
+        <v>4787.8409873832679</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" ref="AC10" si="12">AC9/((1+$B$8)^(AC8-$M$8))</f>
+        <v>4352.5827158029706</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" ref="AD10" si="13">AD9/((1+$B$8)^(AD8-$M$8))</f>
+        <v>3956.8933780027005</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" ref="AE10" si="14">AE9/((1+$B$8)^(AE8-$M$8))</f>
+        <v>3597.1757981842729</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" ref="AF10" si="15">AF9/((1+$B$8)^(AF8-$M$8))</f>
+        <v>3270.1598165311566</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" ref="AG10" si="16">AG9/((1+$B$8)^(AG8-$M$8))</f>
+        <v>2972.8725604828696</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" ref="AH10" si="17">AH9/((1+$B$8)^(AH8-$M$8))</f>
+        <v>2702.6114186207906</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" ref="AI10" si="18">AI9/((1+$B$8)^(AI8-$M$8))</f>
+        <v>2456.9194714734454</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" ref="AJ10" si="19">AJ9/((1+$B$8)^(AJ8-$M$8))</f>
+        <v>2233.56315588495</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" ref="AK10" si="20">AK9/((1+$B$8)^(AK8-$M$8))</f>
+        <v>2030.5119598954095</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" ref="AL10" si="21">AL9/((1+$B$8)^(AL8-$M$8))</f>
+        <v>1845.919963541281</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" ref="AM10" si="22">AM9/((1+$B$8)^(AM8-$M$8))</f>
+        <v>1678.1090577648008</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" ref="AN10" si="23">AN9/((1+$B$8)^(AN8-$M$8))</f>
+        <v>1525.5536888770914</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" ref="AO10" si="24">AO9/((1+$B$8)^(AO8-$M$8))</f>
+        <v>1386.8669898882649</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" ref="AP10" si="25">AP9/((1+$B$8)^(AP8-$M$8))</f>
+        <v>1260.7881726256953</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" ref="AQ10" si="26">AQ9/((1+$B$8)^(AQ8-$M$8))</f>
+        <v>1146.1710660233593</v>
+      </c>
+      <c r="AR10">
+        <f t="shared" ref="AR10" si="27">AR9/((1+$B$8)^(AR8-$M$8))</f>
+        <v>1041.973696384872</v>
+      </c>
+      <c r="AS10">
+        <f t="shared" ref="AS10" si="28">AS9/((1+$B$8)^(AS8-$M$8))</f>
+        <v>947.24881489533823</v>
+      </c>
+      <c r="AT10">
+        <f t="shared" ref="AT10" si="29">AT9/((1+$B$8)^(AT8-$M$8))</f>
+        <v>861.13528626848915</v>
+      </c>
+      <c r="AU10">
+        <f t="shared" ref="AU10" si="30">AU9/((1+$B$8)^(AU8-$M$8))</f>
+        <v>782.85026024408103</v>
+      </c>
+      <c r="AV10">
+        <f t="shared" ref="AV10" si="31">AV9/((1+$B$8)^(AV8-$M$8))</f>
+        <v>711.68205476734624</v>
+      </c>
+      <c r="AW10">
+        <f t="shared" ref="AW10" si="32">AW9/((1+$B$8)^(AW8-$M$8))</f>
+        <v>646.98368615213303</v>
+      </c>
+      <c r="AX10">
+        <f t="shared" ref="AX10" si="33">AX9/((1+$B$8)^(AX8-$M$8))</f>
+        <v>588.16698741102994</v>
+      </c>
+      <c r="AY10">
+        <f t="shared" ref="AY10" si="34">AY9/((1+$B$8)^(AY8-$M$8))</f>
+        <v>534.69726128275443</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" ref="AZ10" si="35">AZ9/((1+$B$8)^(AZ8-$M$8))</f>
+        <v>486.08841934795851</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" ref="BA10" si="36">BA9/((1+$B$8)^(BA8-$M$8))</f>
+        <v>441.8985630435987</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" ref="BB10" si="37">BB9/((1+$B$8)^(BB8-$M$8))</f>
+        <v>401.72596640327151</v>
+      </c>
+      <c r="BC10">
+        <f t="shared" ref="BC10" si="38">BC9/((1+$B$8)^(BC8-$M$8))</f>
+        <v>365.2054240029741</v>
+      </c>
+      <c r="BD10">
+        <f t="shared" ref="BD10" si="39">BD9/((1+$B$8)^(BD8-$M$8))</f>
+        <v>332.00493091179453</v>
+      </c>
+      <c r="BE10">
+        <f t="shared" ref="BE10" si="40">BE9/((1+$B$8)^(BE8-$M$8))</f>
+        <v>301.82266446526779</v>
+      </c>
+      <c r="BF10">
+        <f t="shared" ref="BF10" si="41">BF9/((1+$B$8)^(BF8-$M$8))</f>
+        <v>274.38424042297066</v>
+      </c>
+      <c r="BG10">
+        <f t="shared" ref="BG10" si="42">BG9/((1+$B$8)^(BG8-$M$8))</f>
+        <v>249.44021856633697</v>
+      </c>
+      <c r="BH10">
+        <f t="shared" ref="BH10" si="43">BH9/((1+$B$8)^(BH8-$M$8))</f>
+        <v>226.76383506030632</v>
+      </c>
+      <c r="BI10">
+        <f t="shared" ref="BI10" si="44">BI9/((1+$B$8)^(BI8-$M$8))</f>
+        <v>206.14894096391484</v>
+      </c>
+      <c r="BJ10">
+        <f t="shared" ref="BJ10" si="45">BJ9/((1+$B$8)^(BJ8-$M$8))</f>
+        <v>187.40812814901346</v>
+      </c>
+      <c r="BK10">
+        <f t="shared" ref="BK10" si="46">BK9/((1+$B$8)^(BK8-$M$8))</f>
+        <v>170.37102559001224</v>
+      </c>
+      <c r="BL10">
+        <f t="shared" ref="BL10" si="47">BL9/((1+$B$8)^(BL8-$M$8))</f>
+        <v>154.88275053637474</v>
+      </c>
+      <c r="BM10">
+        <f t="shared" ref="BM10" si="48">BM9/((1+$B$8)^(BM8-$M$8))</f>
+        <v>140.80250048761337</v>
+      </c>
+      <c r="BN10">
+        <f t="shared" ref="BN10" si="49">BN9/((1+$B$8)^(BN8-$M$8))</f>
+        <v>128.0022731705576</v>
+      </c>
+      <c r="BO10">
+        <f t="shared" ref="BO10" si="50">BO9/((1+$B$8)^(BO8-$M$8))</f>
+        <v>116.3657028823251</v>
+      </c>
+      <c r="BP10">
+        <f t="shared" ref="BP10" si="51">BP9/((1+$B$8)^(BP8-$M$8))</f>
+        <v>105.78700262029552</v>
+      </c>
+      <c r="BQ10">
+        <f t="shared" ref="BQ10" si="52">BQ9/((1+$B$8)^(BQ8-$M$8))</f>
+        <v>96.170002382086864</v>
+      </c>
+      <c r="BR10">
+        <f t="shared" ref="BR10" si="53">BR9/((1+$B$8)^(BR8-$M$8))</f>
+        <v>87.427274892806224</v>
+      </c>
+      <c r="BS10">
+        <f t="shared" ref="BS10" si="54">BS9/((1+$B$8)^(BS8-$M$8))</f>
+        <v>79.479340811642018</v>
+      </c>
+      <c r="BT10">
+        <f t="shared" ref="BT10" si="55">BT9/((1+$B$8)^(BT8-$M$8))</f>
+        <v>72.253946192401813</v>
+      </c>
+      <c r="BU10">
+        <f t="shared" ref="BU10" si="56">BU9/((1+$B$8)^(BU8-$M$8))</f>
+        <v>65.685405629456199</v>
+      </c>
+      <c r="BV10">
+        <f t="shared" ref="BV10" si="57">BV9/((1+$B$8)^(BV8-$M$8))</f>
+        <v>59.714005117687449</v>
+      </c>
+      <c r="BW10">
+        <f t="shared" ref="BW10" si="58">BW9/((1+$B$8)^(BW8-$M$8))</f>
+        <v>54.285459197897673</v>
+      </c>
+      <c r="BX10">
+        <f t="shared" ref="BX10" si="59">BX9/((1+$B$8)^(BX8-$M$8))</f>
+        <v>49.350417452634254</v>
+      </c>
+      <c r="BY10">
+        <f t="shared" ref="BY10" si="60">BY9/((1+$B$8)^(BY8-$M$8))</f>
+        <v>44.864015866031131</v>
+      </c>
+      <c r="BZ10">
+        <f t="shared" ref="BZ10" si="61">BZ9/((1+$B$8)^(BZ8-$M$8))</f>
+        <v>40.785468969119208</v>
+      </c>
+      <c r="CA10">
+        <f t="shared" ref="CA10" si="62">CA9/((1+$B$8)^(CA8-$M$8))</f>
+        <v>37.077699062835642</v>
+      </c>
+      <c r="CB10">
+        <f t="shared" ref="CB10" si="63">CB9/((1+$B$8)^(CB8-$M$8))</f>
+        <v>33.706999148032395</v>
+      </c>
+      <c r="CC10">
+        <f t="shared" ref="CC10" si="64">CC9/((1+$B$8)^(CC8-$M$8))</f>
+        <v>30.642726498211271</v>
+      </c>
+      <c r="CD10">
+        <f t="shared" ref="CD10" si="65">CD9/((1+$B$8)^(CD8-$M$8))</f>
+        <v>27.857024089282969</v>
+      </c>
+      <c r="CE10">
+        <f t="shared" ref="CE10" si="66">CE9/((1+$B$8)^(CE8-$M$8))</f>
+        <v>25.324567353893606</v>
+      </c>
+      <c r="CF10">
+        <f t="shared" ref="CF10" si="67">CF9/((1+$B$8)^(CF8-$M$8))</f>
+        <v>23.022333958085095</v>
+      </c>
+      <c r="CG10">
+        <f t="shared" ref="CG10" si="68">CG9/((1+$B$8)^(CG8-$M$8))</f>
+        <v>20.929394507350086</v>
+      </c>
+      <c r="CH10">
+        <f t="shared" ref="CH10" si="69">CH9/((1+$B$8)^(CH8-$M$8))</f>
+        <v>19.026722279409167</v>
+      </c>
+      <c r="CI10">
+        <f t="shared" ref="CI10" si="70">CI9/((1+$B$8)^(CI8-$M$8))</f>
+        <v>17.297020254008334</v>
+      </c>
+      <c r="CJ10">
+        <f t="shared" ref="CJ10" si="71">CJ9/((1+$B$8)^(CJ8-$M$8))</f>
+        <v>15.724563867280303</v>
+      </c>
+      <c r="CK10">
+        <f t="shared" ref="CK10" si="72">CK9/((1+$B$8)^(CK8-$M$8))</f>
+        <v>14.29505806116391</v>
+      </c>
+      <c r="CL10">
+        <f t="shared" ref="CL10" si="73">CL9/((1+$B$8)^(CL8-$M$8))</f>
+        <v>12.995507328330827</v>
+      </c>
+      <c r="CM10">
+        <f t="shared" ref="CM10" si="74">CM9/((1+$B$8)^(CM8-$M$8))</f>
+        <v>11.814097571209841</v>
+      </c>
+      <c r="CN10">
+        <f t="shared" ref="CN10" si="75">CN9/((1+$B$8)^(CN8-$M$8))</f>
+        <v>10.740088701099856</v>
+      </c>
+      <c r="CO10">
+        <f t="shared" ref="CO10" si="76">CO9/((1+$B$8)^(CO8-$M$8))</f>
+        <v>9.7637170009998684</v>
+      </c>
+      <c r="CP10">
+        <f t="shared" ref="CP10" si="77">CP9/((1+$B$8)^(CP8-$M$8))</f>
+        <v>8.8761063645453344</v>
+      </c>
+      <c r="CQ10">
+        <f t="shared" ref="CQ10" si="78">CQ9/((1+$B$8)^(CQ8-$M$8))</f>
+        <v>8.0691876041321215</v>
+      </c>
+      <c r="CR10">
+        <f t="shared" ref="CR10" si="79">CR9/((1+$B$8)^(CR8-$M$8))</f>
+        <v>7.3356250946655628</v>
+      </c>
+      <c r="CS10">
+        <f t="shared" ref="CS10" si="80">CS9/((1+$B$8)^(CS8-$M$8))</f>
+        <v>6.6687500860596041</v>
+      </c>
+      <c r="CT10">
+        <f t="shared" ref="CT10" si="81">CT9/((1+$B$8)^(CT8-$M$8))</f>
+        <v>6.0625000782360026</v>
+      </c>
+      <c r="CU10">
+        <f t="shared" ref="CU10" si="82">CU9/((1+$B$8)^(CU8-$M$8))</f>
+        <v>5.5113637074872743</v>
+      </c>
+      <c r="CV10">
+        <f t="shared" ref="CV10" si="83">CV9/((1+$B$8)^(CV8-$M$8))</f>
+        <v>5.0103306431702492</v>
+      </c>
+      <c r="CW10">
+        <f t="shared" ref="CW10" si="84">CW9/((1+$B$8)^(CW8-$M$8))</f>
+        <v>4.5548460392456818</v>
+      </c>
+      <c r="CX10">
+        <f t="shared" ref="CX10" si="85">CX9/((1+$B$8)^(CX8-$M$8))</f>
+        <v>4.1407691265869824</v>
+      </c>
+      <c r="CY10">
+        <f t="shared" ref="CY10" si="86">CY9/((1+$B$8)^(CY8-$M$8))</f>
+        <v>3.7643355696245293</v>
+      </c>
+      <c r="CZ10">
+        <f t="shared" ref="CZ10" si="87">CZ9/((1+$B$8)^(CZ8-$M$8))</f>
+        <v>3.422123245113208</v>
+      </c>
+      <c r="DA10">
+        <f t="shared" ref="DA10" si="88">DA9/((1+$B$8)^(DA8-$M$8))</f>
+        <v>3.1110211319210981</v>
+      </c>
+      <c r="DB10">
+        <f t="shared" ref="DB10" si="89">DB9/((1+$B$8)^(DB8-$M$8))</f>
+        <v>2.8282010290191799</v>
+      </c>
+      <c r="DC10">
+        <f t="shared" ref="DC10" si="90">DC9/((1+$B$8)^(DC8-$M$8))</f>
+        <v>2.5710918445628903</v>
+      </c>
+      <c r="DD10">
+        <f t="shared" ref="DD10" si="91">DD9/((1+$B$8)^(DD8-$M$8))</f>
+        <v>2.3373562223299005</v>
+      </c>
+      <c r="DE10">
+        <f t="shared" ref="DE10" si="92">DE9/((1+$B$8)^(DE8-$M$8))</f>
+        <v>2.124869293027182</v>
+      </c>
+      <c r="DF10">
+        <f t="shared" ref="DF10" si="93">DF9/((1+$B$8)^(DF8-$M$8))</f>
+        <v>1.9316993572974381</v>
+      </c>
+      <c r="DG10">
+        <f t="shared" ref="DG10" si="94">DG9/((1+$B$8)^(DG8-$M$8))</f>
+        <v>1.7560903248158528</v>
+      </c>
+      <c r="DH10">
+        <f t="shared" ref="DH10" si="95">DH9/((1+$B$8)^(DH8-$M$8))</f>
+        <v>1.5964457498325932</v>
+      </c>
+      <c r="DI10">
+        <f t="shared" ref="DI10" si="96">DI9/((1+$B$8)^(DI8-$M$8))</f>
+        <v>1.4513143180296302</v>
+      </c>
+      <c r="DJ10">
+        <f t="shared" ref="DJ10" si="97">DJ9/((1+$B$8)^(DJ8-$M$8))</f>
+        <v>1.3193766527542092</v>
+      </c>
+      <c r="DK10">
+        <f t="shared" ref="DK10" si="98">DK9/((1+$B$8)^(DK8-$M$8))</f>
+        <v>1.1994333206856445</v>
+      </c>
+      <c r="DL10">
+        <f t="shared" ref="DL10" si="99">DL9/((1+$B$8)^(DL8-$M$8))</f>
+        <v>1.0903939278960404</v>
+      </c>
+      <c r="DM10">
+        <f t="shared" ref="DM10" si="100">DM9/((1+$B$8)^(DM8-$M$8))</f>
+        <v>0.99126720717821848</v>
+      </c>
+      <c r="DN10">
+        <f t="shared" ref="DN10" si="101">DN9/((1+$B$8)^(DN8-$M$8))</f>
+        <v>0.90115200652565319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="39"/>
+      <c r="N11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12">
+        <f>SUM(C10:M10)</f>
+        <v>199990.99999999994</v>
+      </c>
+      <c r="N12">
+        <f>N10</f>
         <v>18181.81818181818</v>
       </c>
-      <c r="R10">
-        <f t="shared" si="0"/>
-        <v>20000</v>
-      </c>
-      <c r="S10">
-        <f>SUM(N10:R10)</f>
-        <v>83397.308926985846</v>
+      <c r="O12">
+        <f>N12+O10</f>
+        <v>34710.74380165289</v>
+      </c>
+      <c r="P12">
+        <f>O12+P10</f>
+        <v>49737.03981968444</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12:CB12" si="102">P12+Q10</f>
+        <v>63397.308926985846</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="102"/>
+        <v>75815.735388168949</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="102"/>
+        <v>87105.213989244497</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="102"/>
+        <v>97368.376353858621</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="102"/>
+        <v>106698.52395805328</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="102"/>
+        <v>115180.47632550297</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="102"/>
+        <v>122891.3421140936</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="102"/>
+        <v>129901.22010372144</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="102"/>
+        <v>136273.83645792858</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="102"/>
+        <v>142067.12405266234</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="102"/>
+        <v>147333.74913878393</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="102"/>
+        <v>152121.5901261672</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="102"/>
+        <v>156474.17284197017</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="102"/>
+        <v>160431.06621997288</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="102"/>
+        <v>164028.24201815715</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="102"/>
+        <v>167298.40183468829</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="102"/>
+        <v>170271.27439517117</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="102"/>
+        <v>172973.88581379197</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="102"/>
+        <v>175430.80528526541</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="102"/>
+        <v>177664.36844115035</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="102"/>
+        <v>179694.88040104575</v>
+      </c>
+      <c r="AL12">
+        <f t="shared" si="102"/>
+        <v>181540.80036458705</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="102"/>
+        <v>183218.90942235186</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="102"/>
+        <v>184744.46311122895</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="102"/>
+        <v>186131.3301011172</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="102"/>
+        <v>187392.1182737429</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="102"/>
+        <v>188538.28933976626</v>
+      </c>
+      <c r="AR12">
+        <f t="shared" si="102"/>
+        <v>189580.26303615113</v>
+      </c>
+      <c r="AS12">
+        <f t="shared" si="102"/>
+        <v>190527.51185104647</v>
+      </c>
+      <c r="AT12">
+        <f t="shared" si="102"/>
+        <v>191388.64713731495</v>
+      </c>
+      <c r="AU12">
+        <f t="shared" si="102"/>
+        <v>192171.49739755903</v>
+      </c>
+      <c r="AV12">
+        <f t="shared" si="102"/>
+        <v>192883.17945232638</v>
+      </c>
+      <c r="AW12">
+        <f t="shared" si="102"/>
+        <v>193530.16313847853</v>
+      </c>
+      <c r="AX12">
+        <f t="shared" si="102"/>
+        <v>194118.33012588957</v>
+      </c>
+      <c r="AY12">
+        <f t="shared" si="102"/>
+        <v>194653.02738717233</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" si="102"/>
+        <v>195139.11580652031</v>
+      </c>
+      <c r="BA12">
+        <f t="shared" si="102"/>
+        <v>195581.0143695639</v>
+      </c>
+      <c r="BB12">
+        <f t="shared" si="102"/>
+        <v>195982.74033596716</v>
+      </c>
+      <c r="BC12">
+        <f t="shared" si="102"/>
+        <v>196347.94575997014</v>
+      </c>
+      <c r="BD12">
+        <f t="shared" si="102"/>
+        <v>196679.95069088193</v>
+      </c>
+      <c r="BE12">
+        <f t="shared" si="102"/>
+        <v>196981.77335534719</v>
+      </c>
+      <c r="BF12">
+        <f t="shared" si="102"/>
+        <v>197256.15759577017</v>
+      </c>
+      <c r="BG12">
+        <f t="shared" si="102"/>
+        <v>197505.59781433651</v>
+      </c>
+      <c r="BH12">
+        <f t="shared" si="102"/>
+        <v>197732.3616493968</v>
+      </c>
+      <c r="BI12">
+        <f t="shared" si="102"/>
+        <v>197938.5105903607</v>
+      </c>
+      <c r="BJ12">
+        <f t="shared" si="102"/>
+        <v>198125.91871850973</v>
+      </c>
+      <c r="BK12">
+        <f t="shared" si="102"/>
+        <v>198296.28974409975</v>
+      </c>
+      <c r="BL12">
+        <f t="shared" si="102"/>
+        <v>198451.17249463612</v>
+      </c>
+      <c r="BM12">
+        <f t="shared" si="102"/>
+        <v>198591.97499512375</v>
+      </c>
+      <c r="BN12">
+        <f t="shared" si="102"/>
+        <v>198719.97726829431</v>
+      </c>
+      <c r="BO12">
+        <f t="shared" si="102"/>
+        <v>198836.34297117664</v>
+      </c>
+      <c r="BP12">
+        <f t="shared" si="102"/>
+        <v>198942.12997379692</v>
+      </c>
+      <c r="BQ12">
+        <f t="shared" si="102"/>
+        <v>199038.299976179</v>
+      </c>
+      <c r="BR12">
+        <f t="shared" si="102"/>
+        <v>199125.7272510718</v>
+      </c>
+      <c r="BS12">
+        <f t="shared" si="102"/>
+        <v>199205.20659188344</v>
+      </c>
+      <c r="BT12">
+        <f t="shared" si="102"/>
+        <v>199277.46053807583</v>
+      </c>
+      <c r="BU12">
+        <f t="shared" si="102"/>
+        <v>199343.14594370528</v>
+      </c>
+      <c r="BV12">
+        <f t="shared" si="102"/>
+        <v>199402.85994882297</v>
+      </c>
+      <c r="BW12">
+        <f t="shared" si="102"/>
+        <v>199457.14540802088</v>
+      </c>
+      <c r="BX12">
+        <f t="shared" si="102"/>
+        <v>199506.49582547351</v>
+      </c>
+      <c r="BY12">
+        <f t="shared" si="102"/>
+        <v>199551.35984133955</v>
+      </c>
+      <c r="BZ12">
+        <f t="shared" si="102"/>
+        <v>199592.14531030867</v>
+      </c>
+      <c r="CA12">
+        <f t="shared" si="102"/>
+        <v>199629.22300937149</v>
+      </c>
+      <c r="CB12">
+        <f t="shared" si="102"/>
+        <v>199662.93000851953</v>
+      </c>
+      <c r="CC12">
+        <f t="shared" ref="CC12:DN12" si="103">CB12+CC10</f>
+        <v>199693.57273501775</v>
+      </c>
+      <c r="CD12">
+        <f t="shared" si="103"/>
+        <v>199721.42975910704</v>
+      </c>
+      <c r="CE12">
+        <f t="shared" si="103"/>
+        <v>199746.75432646094</v>
+      </c>
+      <c r="CF12">
+        <f t="shared" si="103"/>
+        <v>199769.77666041904</v>
+      </c>
+      <c r="CG12">
+        <f t="shared" si="103"/>
+        <v>199790.70605492638</v>
+      </c>
+      <c r="CH12">
+        <f t="shared" si="103"/>
+        <v>199809.73277720579</v>
+      </c>
+      <c r="CI12">
+        <f t="shared" si="103"/>
+        <v>199827.02979745981</v>
+      </c>
+      <c r="CJ12">
+        <f t="shared" si="103"/>
+        <v>199842.7543613271</v>
+      </c>
+      <c r="CK12">
+        <f t="shared" si="103"/>
+        <v>199857.04941938826</v>
+      </c>
+      <c r="CL12">
+        <f t="shared" si="103"/>
+        <v>199870.0449267166</v>
+      </c>
+      <c r="CM12">
+        <f t="shared" si="103"/>
+        <v>199881.85902428781</v>
+      </c>
+      <c r="CN12">
+        <f t="shared" si="103"/>
+        <v>199892.59911298892</v>
+      </c>
+      <c r="CO12">
+        <f t="shared" si="103"/>
+        <v>199902.36282998993</v>
+      </c>
+      <c r="CP12">
+        <f t="shared" si="103"/>
+        <v>199911.23893635446</v>
+      </c>
+      <c r="CQ12">
+        <f t="shared" si="103"/>
+        <v>199919.30812395859</v>
+      </c>
+      <c r="CR12">
+        <f t="shared" si="103"/>
+        <v>199926.64374905324</v>
+      </c>
+      <c r="CS12">
+        <f t="shared" si="103"/>
+        <v>199933.31249913931</v>
+      </c>
+      <c r="CT12">
+        <f t="shared" si="103"/>
+        <v>199939.37499921754</v>
+      </c>
+      <c r="CU12">
+        <f t="shared" si="103"/>
+        <v>199944.88636292503</v>
+      </c>
+      <c r="CV12">
+        <f t="shared" si="103"/>
+        <v>199949.89669356821</v>
+      </c>
+      <c r="CW12">
+        <f t="shared" si="103"/>
+        <v>199954.45153960746</v>
+      </c>
+      <c r="CX12">
+        <f t="shared" si="103"/>
+        <v>199958.59230873405</v>
+      </c>
+      <c r="CY12">
+        <f t="shared" si="103"/>
+        <v>199962.35664430368</v>
+      </c>
+      <c r="CZ12">
+        <f t="shared" si="103"/>
+        <v>199965.77876754879</v>
+      </c>
+      <c r="DA12">
+        <f t="shared" si="103"/>
+        <v>199968.88978868071</v>
+      </c>
+      <c r="DB12">
+        <f t="shared" si="103"/>
+        <v>199971.71798970972</v>
+      </c>
+      <c r="DC12">
+        <f t="shared" si="103"/>
+        <v>199974.28908155428</v>
+      </c>
+      <c r="DD12">
+        <f t="shared" si="103"/>
+        <v>199976.62643777661</v>
+      </c>
+      <c r="DE12">
+        <f t="shared" si="103"/>
+        <v>199978.75130706964</v>
+      </c>
+      <c r="DF12">
+        <f t="shared" si="103"/>
+        <v>199980.68300642693</v>
+      </c>
+      <c r="DG12">
+        <f t="shared" si="103"/>
+        <v>199982.43909675174</v>
+      </c>
+      <c r="DH12">
+        <f t="shared" si="103"/>
+        <v>199984.03554250157</v>
+      </c>
+      <c r="DI12">
+        <f t="shared" si="103"/>
+        <v>199985.4868568196</v>
+      </c>
+      <c r="DJ12">
+        <f t="shared" si="103"/>
+        <v>199986.80623347234</v>
+      </c>
+      <c r="DK12">
+        <f t="shared" si="103"/>
+        <v>199988.00566679303</v>
+      </c>
+      <c r="DL12">
+        <f t="shared" si="103"/>
+        <v>199989.09606072094</v>
+      </c>
+      <c r="DM12">
+        <f t="shared" si="103"/>
+        <v>199990.08732792811</v>
+      </c>
+      <c r="DN12">
+        <f t="shared" si="103"/>
+        <v>199990.98847993463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13">
+        <f>SUM(N10:DN10)</f>
+        <v>199990.98847993463</v>
+      </c>
+      <c r="N13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2">
+        <v>10792.142736644701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16">
+        <f>$B$17</f>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:M16" si="104">$B$17</f>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="104"/>
+        <v>10294.278788325608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10294.278788325608</v>
+      </c>
+      <c r="C17">
+        <f>C16*(1+$B$8)^($M$8-C8)</f>
+        <v>26700.707989386927</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:M17" si="105">D16*(1+$B$8)^($M$8-D8)</f>
+        <v>24273.37089944266</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="105"/>
+        <v>22066.700817675144</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="105"/>
+        <v>20060.637106977403</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="105"/>
+        <v>18236.942824524911</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="105"/>
+        <v>16579.03893138628</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="105"/>
+        <v>15071.853573987526</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="105"/>
+        <v>13701.685067261387</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="105"/>
+        <v>12456.077333873987</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="105"/>
+        <v>11323.706667158169</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="105"/>
+        <v>10294.278788325608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18">
+        <f>SUM(C17:M17)</f>
+        <v>190765.00000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19">
+        <v>190765</v>
       </c>
     </row>
   </sheetData>
@@ -4461,42 +7379,42 @@
   <sheetData>
     <row r="8" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>1000</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="H8" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="38" t="s">
+      <c r="J8" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="38" t="s">
+      <c r="K8" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="L8" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="L8" s="38" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -4604,7 +7522,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E11:E13" si="3">L11</f>
+        <f t="shared" ref="E12:E13" si="3">L11</f>
         <v>600</v>
       </c>
       <c r="F12" s="5">
@@ -4691,39 +7609,39 @@
   <sheetData>
     <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>10000</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="G6" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="38" t="s">
+      <c r="I6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="J6" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="K6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="L6" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="L6" s="38" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -4752,7 +7670,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1">
         <v>0.15</v>
@@ -4825,22 +7743,22 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F9:F12" si="2">L9</f>
+        <f t="shared" ref="F10:F12" si="2">L9</f>
         <v>6811.2156220771394</v>
       </c>
       <c r="G10" s="1">
         <v>0.15</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H9:H12" si="3">F10*G10</f>
+        <f t="shared" ref="H10:H12" si="3">F10*G10</f>
         <v>1021.6823433115709</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I9:I12" si="4">H10</f>
+        <f t="shared" ref="I10:I12" si="4">H10</f>
         <v>1021.6823433115709</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J9:J12" si="5">K10-I10</f>
+        <f t="shared" ref="J10:J12" si="5">K10-I10</f>
         <v>1961.4731813037133</v>
       </c>
       <c r="K10">
@@ -4923,7 +7841,7 @@
         <v>-6.3664629124104977E-12</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4948,29 +7866,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="38" t="s">
+      <c r="H6" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="I6" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="J6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="K6" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -5002,7 +7920,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>10000</v>
@@ -5041,7 +7959,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -5080,7 +7998,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1">
         <v>0.15</v>
@@ -5212,44 +8130,44 @@
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>10000</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="38" t="s">
+      <c r="H5" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="I5" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="J5" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="K5" s="36" t="s">
         <v>49</v>
-      </c>
-      <c r="K5" s="38" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5281,7 +8199,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1">
         <v>0.12</v>
@@ -5301,7 +8219,7 @@
         <f>E7*F7</f>
         <v>1200</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="37">
         <v>1200</v>
       </c>
       <c r="I7">
@@ -5390,7 +8308,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -5478,7 +8396,7 @@
   <sheetData>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -5495,7 +8413,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5514,7 +8432,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1">
         <v>0.18</v>
@@ -5543,9 +8461,9 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="36">
+        <v>60</v>
+      </c>
+      <c r="D14" s="34">
         <f>((1+D12)/(1+D13))-1</f>
         <v>0.1132075471698113</v>
       </c>
@@ -5559,7 +8477,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -5580,37 +8498,368 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A782090-6A1E-43FD-AEE4-111472A01453}">
-  <dimension ref="A6:B8"/>
+  <dimension ref="A6:AB16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <f>B7/12</f>
         <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="C8">
+        <f>0.1/12</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" s="33">
+        <v>8.3332999999999996E-5</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>11</v>
+      </c>
+      <c r="P9">
+        <v>12</v>
+      </c>
+      <c r="Q9">
+        <v>13</v>
+      </c>
+      <c r="R9">
+        <v>14</v>
+      </c>
+      <c r="S9">
+        <v>15</v>
+      </c>
+      <c r="T9">
+        <v>16</v>
+      </c>
+      <c r="U9">
+        <v>17</v>
+      </c>
+      <c r="V9">
+        <v>18</v>
+      </c>
+      <c r="W9">
+        <v>19</v>
+      </c>
+      <c r="X9">
+        <v>20</v>
+      </c>
+      <c r="Y9">
+        <v>21</v>
+      </c>
+      <c r="Z9">
+        <v>22</v>
+      </c>
+      <c r="AA9">
+        <v>23</v>
+      </c>
+      <c r="AB9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <f>$C$13</f>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:AB10" si="0">$C$13</f>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="Y10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="Z10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="AA10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+      <c r="AB10" s="2">
+        <f t="shared" si="0"/>
+        <v>88.218924213350277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f>D10*(1+$B$8)^($AB$9-D9)</f>
+        <v>107.66157773224813</v>
+      </c>
+      <c r="E11">
+        <f>E10*(1+$B$8)^($AB$9-E9)</f>
+        <v>106.77181262702294</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="E11:AB11" si="1">F10*(1+$B$8)^($AB$9-F9)</f>
+        <v>105.88940095241946</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>105.01428193628374</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>104.14639530871116</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>103.28568129789538</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>102.43208062601197</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>101.58553450513581</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>100.74598463319255</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>99.91337318994303</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>99.087642833001354</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>98.268736693885629</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>97.456598374101475</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>96.651171941257658</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>95.85240192521421</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>95.060233314262035</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>94.27461155133426</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>93.495482530248836</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="1"/>
+        <v>92.722792591982341</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>91.956488520974204</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="1"/>
+        <v>91.196517541462029</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="1"/>
+        <v>90.442827313846649</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>89.695365931087593</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="1"/>
+        <v>88.954081915128199</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="1"/>
+        <v>88.218924213350277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13">
+        <v>88.218924213350277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15">
+        <f>SUM(D11:AB11)</f>
+        <v>2440.7800000000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <f>B6*(1+B8)^(24)</f>
+        <v>2440.7819227511181</v>
       </c>
     </row>
   </sheetData>
@@ -5648,9 +8897,9 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="35">
+        <v>55</v>
+      </c>
+      <c r="B7" s="33">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="C7" s="2">
@@ -5719,7 +8968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3884B2-0C0A-4FC7-AD0F-165867150FEB}">
   <dimension ref="A7:BX18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -5727,7 +8976,7 @@
   <sheetData>
     <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>2000</v>
@@ -5759,7 +9008,7 @@
     </row>
     <row r="8" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1">
         <v>0.04</v>
@@ -5791,7 +9040,7 @@
     </row>
     <row r="9" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9">
         <f>B8/12</f>
@@ -5801,7 +9050,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:76" x14ac:dyDescent="0.25">
@@ -5809,15 +9058,15 @@
         <v>5000</v>
       </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -6040,7 +9289,7 @@
       </c>
     </row>
     <row r="13" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
+      <c r="A13" s="33">
         <v>3.3E-3</v>
       </c>
       <c r="B13">
@@ -6641,7 +9890,7 @@
     </row>
     <row r="16" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16">
         <v>29.913456439437823</v>
@@ -6652,7 +9901,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17">
         <f>SUM(D14:BX14)</f>
@@ -6661,7 +9910,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18">
         <f>5000-B7*(1+A13)^(B13)</f>
@@ -6915,7 +10164,7 @@
         <v>45.454545454545453</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O12:O19" si="4">SUM(J14:N14)</f>
+        <f t="shared" ref="O14:O19" si="4">SUM(J14:N14)</f>
         <v>439.45454545454544</v>
       </c>
     </row>
@@ -7172,7 +10421,7 @@
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -7268,7 +10517,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -7282,7 +10531,7 @@
   <dimension ref="A2:N14"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7374,7 +10623,7 @@
         <v>47.619047619047613</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" ref="J6:M6" si="0">D6/((1+$A$6)^(3))</f>
+        <f t="shared" ref="K6:M6" si="0">D6/((1+$A$6)^(3))</f>
         <v>90.702947845804985</v>
       </c>
       <c r="L6" s="9">
@@ -7898,7 +11147,7 @@
         <v>0.15</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" ref="I11:I15" si="2">1/((1+C12)^(I11-$H$9))</f>
+        <f t="shared" ref="I12:I15" si="2">1/((1+C12)^(I11-$H$9))</f>
         <v>0.82158574326292821</v>
       </c>
       <c r="J12" s="9">
@@ -8024,7 +11273,7 @@
   <dimension ref="B2:O20"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,42 +11318,41 @@
       <c r="I4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18">
+      <c r="K4">
         <v>1250</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4">
         <v>1500</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4">
         <v>1750</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="18">
         <v>2000</v>
       </c>
     </row>
     <row r="5" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21">
+      <c r="J5" s="20"/>
+      <c r="K5" s="20">
         <f>K4/((1+K3)^(K2))</f>
         <v>1136.3636363636363</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="20">
         <f>L4/((1+K3)*(1+L3))</f>
         <v>1185.7707509881425</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="20">
         <f>M4/((1+K3)*(1+L3)*(1+M3))</f>
         <v>1152.8326745718052</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="21">
         <f>N4/((1+K3)*(1+L3)*(1+M3)*(1+N3))</f>
         <v>1054.0184453227932</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5">
         <f>SUM(K5:N5)</f>
         <v>4528.985507246377</v>
       </c>
@@ -8149,48 +11397,48 @@
       <c r="I9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9">
         <v>-4200</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9">
         <v>1250</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9">
         <v>1500</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9">
         <v>1750</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="18">
         <v>2000</v>
       </c>
     </row>
     <row r="10" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="20">
         <v>-4200</v>
       </c>
-      <c r="K10" s="21">
-        <f>K9/((1+K8)^(K7))</f>
+      <c r="K10" s="20">
+        <f>K9/(1+K8)</f>
         <v>1000</v>
       </c>
-      <c r="L10" s="21">
-        <f t="shared" ref="L10:N10" si="0">L9/((1+L8)^(L7))</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="M10" s="21">
-        <f t="shared" si="0"/>
-        <v>1150.6534067559796</v>
-      </c>
-      <c r="N10" s="22">
-        <f>N9/((1+N8)^(N7))</f>
-        <v>1366.026910730141</v>
-      </c>
-      <c r="O10" s="24">
+      <c r="L10" s="20">
+        <f>L9/((1+L8)*(1+K8))</f>
+        <v>1000</v>
+      </c>
+      <c r="M10" s="20">
+        <f>M9/((1+M8)*(1+L8)*(1+K8))</f>
+        <v>1014.4927536231885</v>
+      </c>
+      <c r="N10" s="21">
+        <f>N9/((1+N8)*(1+M8)*(1+L8)*(1+K8))</f>
+        <v>1054.0184453227932</v>
+      </c>
+      <c r="O10">
         <f>SUM(J10:N10)</f>
-        <v>358.34698415278763</v>
+        <v>-131.48880105401827</v>
       </c>
     </row>
     <row r="12" spans="9:15" x14ac:dyDescent="0.25">
@@ -8233,48 +11481,48 @@
       <c r="I14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14">
         <v>-4200</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14">
         <v>1250</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14">
         <v>1500</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14">
         <v>1750</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="18">
         <v>2000</v>
       </c>
     </row>
     <row r="15" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="20">
         <v>-4200</v>
       </c>
-      <c r="K15" s="21">
+      <c r="K15" s="20">
         <f>K14/((1+K13)^(K12))</f>
         <v>1077.5862068965519</v>
       </c>
-      <c r="L15" s="21">
-        <f t="shared" ref="L15:N15" si="1">L14/((1+L13)^(L12))</f>
-        <v>1154.2012927054475</v>
-      </c>
-      <c r="M15" s="21">
-        <f t="shared" si="1"/>
-        <v>1245.6154336734689</v>
-      </c>
-      <c r="N15" s="22">
-        <f t="shared" si="1"/>
-        <v>1366.026910730141</v>
-      </c>
-      <c r="O15" s="24">
+      <c r="L15" s="20">
+        <f>L14/((1+L13)*(1+K13))</f>
+        <v>1134.3012704174228</v>
+      </c>
+      <c r="M15" s="20">
+        <f>M14/((1+M13)*(1+L13)*(1+K13))</f>
+        <v>1181.5638233514819</v>
+      </c>
+      <c r="N15" s="21">
+        <f>N14/((1+N13)*(1+M13)*(1+L13)*(1+K13))</f>
+        <v>1227.5987775080332</v>
+      </c>
+      <c r="O15">
         <f>SUM(J15:N15)</f>
-        <v>643.42984400560908</v>
+        <v>421.05007817348951</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -8320,48 +11568,48 @@
       <c r="I19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19">
         <v>-3000</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19">
         <v>1750</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19">
         <v>2500</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19">
         <v>-500</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N19" s="18">
         <v>875</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="20">
         <v>-3000</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="20">
         <f>K19/((1+K18)^(K17))</f>
         <v>1521.7391304347827</v>
       </c>
-      <c r="L20" s="21">
-        <f t="shared" ref="L20:N20" si="2">L19/((1+L18)^(L17))</f>
-        <v>2066.1157024793383</v>
-      </c>
-      <c r="M20" s="21">
-        <f t="shared" si="2"/>
-        <v>-375.65740045078877</v>
-      </c>
-      <c r="N20" s="22">
-        <f t="shared" si="2"/>
-        <v>597.6367734444367</v>
-      </c>
-      <c r="O20" s="24">
+      <c r="L20" s="20">
+        <f>L19/((1+L18)*(1+K18))</f>
+        <v>1976.2845849802372</v>
+      </c>
+      <c r="M20" s="20">
+        <f>M19/((1+M18)*(1+L18)*(1+K18))</f>
+        <v>-359.32446999640672</v>
+      </c>
+      <c r="N20" s="21">
+        <f>N19/((1+N18)*(1+M18)*(1+L18)*(1+K18))</f>
+        <v>571.65256590337424</v>
+      </c>
+      <c r="O20">
         <f>SUM(J20:N20)</f>
-        <v>809.83420590776905</v>
+        <v>710.3518113219875</v>
       </c>
     </row>
   </sheetData>
@@ -8452,7 +11700,7 @@
         <v>0.7561436672967865</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" ref="E11:G11" si="0">1/((1+F10)^(F8))</f>
+        <f t="shared" ref="F11:G11" si="0">1/((1+F10)^(F8))</f>
         <v>0.65751623243198831</v>
       </c>
       <c r="G11" s="9">
@@ -8477,7 +11725,7 @@
         <v>1643.7905810799707</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="E12:G12" si="1">G9*G11</f>
+        <f t="shared" ref="G12" si="1">G9*G11</f>
         <v>1429.3831139825836</v>
       </c>
       <c r="H12">
@@ -8579,7 +11827,7 @@
         <v>0.69444444444444442</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:G10" si="0">1/((1+F9)^(F7))</f>
+        <f t="shared" ref="F10" si="0">1/((1+F9)^(F7))</f>
         <v>0.57870370370370372</v>
       </c>
       <c r="G10">
@@ -8704,7 +11952,7 @@
         <v>1890.3591682419662</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="E11:G11" si="0">F9/((1+F10)^(F8))</f>
+        <f t="shared" ref="F11:G11" si="0">F9/((1+F10)^(F8))</f>
         <v>1643.7905810799709</v>
       </c>
       <c r="G11">

</xml_diff>

<commit_message>
notes from sessions and ex on week5
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week3/hw1.xlsx
+++ b/PM2/econ/week3/hw1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E816F9DB-C584-4451-8EE9-0744C554A49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CFFD6F-7CD0-4309-A3CC-7AD0DDE984D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="15" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="24" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
   </bookViews>
   <sheets>
     <sheet name="ex1g" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,19 @@
     <sheet name="ex14g" sheetId="14" r:id="rId14"/>
     <sheet name="ex15g" sheetId="15" r:id="rId15"/>
     <sheet name="ex16" sheetId="16" r:id="rId16"/>
-    <sheet name="ex17" sheetId="17" r:id="rId17"/>
+    <sheet name="ex17g" sheetId="17" r:id="rId17"/>
     <sheet name="ex18" sheetId="18" r:id="rId18"/>
     <sheet name="ex19b" sheetId="19" r:id="rId19"/>
-    <sheet name="ex20" sheetId="20" r:id="rId20"/>
-    <sheet name="ex21" sheetId="21" r:id="rId21"/>
-    <sheet name="ex22" sheetId="22" r:id="rId22"/>
+    <sheet name="ex20g" sheetId="20" r:id="rId20"/>
+    <sheet name="ex21g" sheetId="21" r:id="rId21"/>
+    <sheet name="ex22g" sheetId="22" r:id="rId22"/>
     <sheet name="ex23" sheetId="23" r:id="rId23"/>
-    <sheet name="ex24" sheetId="24" r:id="rId24"/>
-    <sheet name="ex25" sheetId="25" r:id="rId25"/>
+    <sheet name="ex24g" sheetId="24" r:id="rId24"/>
+    <sheet name="ex25g" sheetId="25" r:id="rId25"/>
     <sheet name="ex26b" sheetId="26" r:id="rId26"/>
-    <sheet name="ex27" sheetId="27" r:id="rId27"/>
+    <sheet name="ex27g" sheetId="27" r:id="rId27"/>
     <sheet name="ex28" sheetId="28" r:id="rId28"/>
-    <sheet name="ex29" sheetId="29" r:id="rId29"/>
+    <sheet name="ex29g" sheetId="29" r:id="rId29"/>
     <sheet name="ex30" sheetId="30" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="121">
   <si>
     <t>Flujos</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>Valores en el año 3</t>
-  </si>
-  <si>
-    <t>Traerlo todo del 3 al 0</t>
   </si>
   <si>
     <t>celda fija</t>
@@ -305,6 +302,132 @@
   </si>
   <si>
     <t>definición de flujo aquí</t>
+  </si>
+  <si>
+    <t>flujo es toda la tabla, un flujo está compuesto de varios momentos</t>
+  </si>
+  <si>
+    <t>valor f o p al 3 es valor equivalente al 3</t>
+  </si>
+  <si>
+    <t>no pide la suma</t>
+  </si>
+  <si>
+    <t>o Traerlo todo del 3 al 0</t>
+  </si>
+  <si>
+    <t>del 0 al 1 es 10%</t>
+  </si>
+  <si>
+    <t>INF</t>
+  </si>
+  <si>
+    <t>((1+TN)/(1+TR))-1</t>
+  </si>
+  <si>
+    <t>Índice de precios = factor de acumulación</t>
+  </si>
+  <si>
+    <t>la tasa promedio daría 1.1686 al saltar 3</t>
+  </si>
+  <si>
+    <t>el 1.1686 es igual a (1+r)^(3), la r es la tasa promedio de cómo creció ese</t>
+  </si>
+  <si>
+    <t>para dar varios brincos en uno, necesitas tasas iguales</t>
+  </si>
+  <si>
+    <t>del año 0 al 1 la inf es 5%</t>
+  </si>
+  <si>
+    <t>el 0 vale 1, los siguientes es sacar cuanto vale ese peso en el futuro, o el factor</t>
+  </si>
+  <si>
+    <t>correcto</t>
+  </si>
+  <si>
+    <t>despejas r</t>
+  </si>
+  <si>
+    <t>determinar el incremento en el precio cada año</t>
+  </si>
+  <si>
+    <t>te podrían decir que ese incremento se dio en 5 años y saques el inc del p cada año</t>
+  </si>
+  <si>
+    <t>es este</t>
+  </si>
+  <si>
+    <t>del 2009 al 2010 es 6.5%</t>
+  </si>
+  <si>
+    <t>traerlo al 2009</t>
+  </si>
+  <si>
+    <t>indice de precios (tasas acumuladas)</t>
+  </si>
+  <si>
+    <t>saca la tasa nominal</t>
+  </si>
+  <si>
+    <t>Vf</t>
+  </si>
+  <si>
+    <t>Vp</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>tasa promedio de la inflación</t>
+  </si>
+  <si>
+    <t>tasa promedio del aumento de sueldo</t>
+  </si>
+  <si>
+    <t>la tasa real</t>
+  </si>
+  <si>
+    <t>comprobando</t>
+  </si>
+  <si>
+    <t>empieza a recibir la lana a partir del 21, anualidades vencidas</t>
+  </si>
+  <si>
+    <t>en el año 20 recibir es anualidades anticipadas, pero no recibes en 40 (20 pagos exactos)</t>
+  </si>
+  <si>
+    <t>pagos vencidos</t>
+  </si>
+  <si>
+    <t>VP = A / r</t>
+  </si>
+  <si>
+    <t>200k para el año 11, y con solver</t>
+  </si>
+  <si>
+    <t>ahorro desde hoy (anticipado) es 11408</t>
+  </si>
+  <si>
+    <t>vencido (ahorras desde el 1) es 12549</t>
+  </si>
+  <si>
+    <t>con 200, el primer mes genera 20, y asi perpetuamente</t>
+  </si>
+  <si>
+    <t>Hoy tengo 25, si planeo vivir hasta los 80 años, y retirarme a los 40 años, cuanto debo de ahorrar para sacar 30 años cuando me retire (vencido)</t>
+  </si>
+  <si>
+    <t>anual</t>
+  </si>
+  <si>
+    <t>ahorro</t>
+  </si>
+  <si>
+    <t>Disposición</t>
+  </si>
+  <si>
+    <t>también puedes asumir gracia de capital y de interés</t>
   </si>
 </sst>
 </file>
@@ -529,7 +652,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -558,11 +681,6 @@
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
@@ -571,6 +689,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -689,7 +813,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'ex21'!$N$12:$DN$12</c:f>
+              <c:f>ex21g!$N$12:$DN$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="105"/>
@@ -3761,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3AA9C7-6482-4635-B617-27F45774E45F}">
-  <dimension ref="B12:I25"/>
+  <dimension ref="B5:K25"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,7 +3896,12 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
@@ -3798,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
@@ -3819,7 +3948,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -3844,7 +3973,7 @@
         <v>449.38125000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -3863,7 +3992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -4049,7 +4178,7 @@
         <v>1200</v>
       </c>
       <c r="G23" s="4">
-        <v>750</v>
+        <v>-750</v>
       </c>
       <c r="H23" s="4">
         <v>1000</v>
@@ -4073,7 +4202,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>1012.5000000000001</v>
+        <v>-1012.5000000000001</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
@@ -4081,7 +4210,7 @@
       </c>
       <c r="I24">
         <f>SUM(D24:H24)</f>
-        <v>447.42812499999911</v>
+        <v>-1577.571875000001</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -4090,7 +4219,7 @@
       </c>
       <c r="I25">
         <f>SUM(I14:I24)</f>
-        <v>507.90614500000027</v>
+        <v>-1517.0938549999998</v>
       </c>
     </row>
   </sheetData>
@@ -4105,14 +4234,14 @@
   <dimension ref="B7:H10"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -4135,7 +4264,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4">
         <v>10000</v>
@@ -4155,7 +4284,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>0</v>
@@ -4177,27 +4306,27 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <f>C8/((1+C9)^(C7))</f>
         <v>10000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f>D8/((1+D9)^(D7))</f>
         <v>8333.3333333333339</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" ref="E10:G10" si="0">E8/((1+E9)^(E7))</f>
         <v>6944.4444444444443</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>5787.0370370370374</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>4822.5308641975307</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <f>SUM(C10:G10)</f>
         <v>35887.345679012345</v>
       </c>
@@ -4210,10 +4339,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AD0BC3-834A-4A18-AF43-097DA6D42139}">
-  <dimension ref="B8:G11"/>
+  <dimension ref="B8:G14"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,7 +4355,7 @@
   <sheetData>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>2</v>
@@ -4246,14 +4375,14 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="23">
         <v>0.15</v>
       </c>
-      <c r="D9" s="29">
-        <f>(D11/D10)-1</f>
-        <v>0.66666666666666674</v>
+      <c r="D9" s="38">
+        <f>((D11+1)/(D10+1))-1</f>
+        <v>8.6956521739130599E-2</v>
       </c>
       <c r="E9" s="23">
         <v>0.15</v>
@@ -4267,7 +4396,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="25">
         <v>0.1</v>
@@ -4275,23 +4404,23 @@
       <c r="D10" s="25">
         <v>0.15</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <f>((1+E11)/(1+E9))-1</f>
         <v>8.6956521739130599E-2</v>
       </c>
       <c r="F10" s="25">
         <v>0.15</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="37">
         <f>((1+G11)/(1+G9))-1</f>
         <v>8.0000000000000071E-2</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="28">
+        <v>28</v>
+      </c>
+      <c r="C11" s="35">
         <f>(1+C10)*(1+C9)-1</f>
         <v>0.2649999999999999</v>
       </c>
@@ -4301,12 +4430,20 @@
       <c r="E11" s="26">
         <v>0.25</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="36">
         <f>(1+F10)*(1+F9)-1</f>
         <v>0.55249999999999999</v>
       </c>
       <c r="G11" s="27">
         <v>0.35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4317,17 +4454,17 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192EA878-C13A-42CA-8D97-21D9F7ED6C14}">
-  <dimension ref="B6:E10"/>
+  <dimension ref="B6:K17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4339,37 +4476,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>0.05</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="28">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="28">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8">
-        <v>105</v>
-      </c>
-      <c r="D8" s="33"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>106.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>104.5</v>
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="D8" s="39">
+        <v>1.1183000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.1686000000000001</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -4400,14 +4560,14 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="33"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="1">
         <v>0.05</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="28">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="28">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
@@ -4436,36 +4596,69 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9295E89-FDF5-4CD3-B6BC-0D882F1A91E9}">
-  <dimension ref="C6:D9"/>
+  <dimension ref="C6:G14"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3500</v>
       </c>
       <c r="D7">
         <v>4375</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="3">
         <f>(D7-C7)/3500</f>
+        <v>0.25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.25</v>
       </c>
     </row>
@@ -4480,7 +4673,7 @@
   <dimension ref="C6:D9"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4490,7 +4683,7 @@
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1">
         <v>0.15</v>
@@ -4498,7 +4691,7 @@
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1">
         <v>0.25</v>
@@ -4506,9 +4699,9 @@
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="34">
+        <v>32</v>
+      </c>
+      <c r="D9" s="29">
         <f>((1+D7)/(1+D6))-1</f>
         <v>8.6956521739130599E-2</v>
       </c>
@@ -4523,15 +4716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A87A3C-FCF6-4DCA-8556-96ABD2ECB3FE}">
   <dimension ref="B6:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6">
         <v>5500</v>
@@ -4539,7 +4732,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>0.15</v>
@@ -4547,11 +4740,11 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
-        <f>550/((1+C7))</f>
-        <v>478.26086956521743</v>
+        <f>5500/((1+C7))</f>
+        <v>4782.608695652174</v>
       </c>
     </row>
   </sheetData>
@@ -4562,15 +4755,20 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A0A834-9DCB-4AE7-BAAC-CA4F11D6D108}">
-  <dimension ref="B9:I11"/>
+  <dimension ref="B6:L36"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6">
         <v>2009</v>
@@ -4585,12 +4783,12 @@
         <v>2012</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4">
         <v>11809.7</v>
@@ -4606,22 +4804,25 @@
       <c r="F10" s="4">
         <v>25666.5</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <f>F10/((1+D11)*(1+E11)*(1+F11))</f>
         <v>22389.446302489781</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="35">
+        <v>30</v>
+      </c>
+      <c r="C11" s="30">
         <v>0</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="30">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="30">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F11" s="1">
@@ -4632,7 +4833,140 @@
         <v>1.8958522487861487</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="E14">
+        <v>1.1023000000000001</v>
+      </c>
+      <c r="F14">
+        <v>1.1464000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18">
+        <v>25666.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19">
+        <v>11809.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <f>(C18/C19)^(1/3)-1</f>
+        <v>0.29531659130632826</v>
+      </c>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24">
+        <f>E10*(1+F11)</f>
+        <v>13538.2385502</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25">
+        <v>11809.7</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <f>(C24/C25)^(1/C26)-1</f>
+        <v>4.6584822374098778E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <f>(1+C21)/(1+C27)-1</f>
+        <v>0.23766040134998345</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <f>C10*(1+C21)^(3)</f>
+        <v>25666.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <f>C10*(1+C27)^(3)</f>
+        <v>13538.238550200003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <f>C10*(1+B31)^(3)</f>
+        <v>22389.44630248977</v>
       </c>
     </row>
   </sheetData>
@@ -4646,7 +4980,7 @@
   <dimension ref="A5:C7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4673,7 +5007,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>0.25</v>
@@ -4687,10 +5021,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402C4898-B0EB-42D7-B24C-7FAE7772AC8D}">
-  <dimension ref="B9:F12"/>
+  <dimension ref="B9:F17"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4719,7 +5053,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>250</v>
@@ -4730,11 +5064,47 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <f>C9/C10-1</f>
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <f>C9/(1+C15)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <f>C9/(1+C16)</f>
+        <v>961.53846153846155</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <f>C9/(1+C17)</f>
+        <v>1086.9565217391305</v>
       </c>
     </row>
   </sheetData>
@@ -4745,10 +5115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3841B5-E01A-4CC0-9035-2C30A4D4C700}">
-  <dimension ref="B15:P24"/>
+  <dimension ref="B15:Q24"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView topLeftCell="D7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,12 +5219,12 @@
         <f>H16/((1+$C$16)^(O15-$K$15))</f>
         <v>123.40537121878229</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="34">
         <f>SUM(K16:O16)</f>
         <v>369.7070665000694</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -4899,12 +5269,12 @@
         <f t="shared" si="1"/>
         <v>25.728896051686501</v>
       </c>
-      <c r="P17" s="9">
+      <c r="P17" s="34">
         <f>SUM(K17:O17)</f>
         <v>71.541339546385288</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
@@ -4949,12 +5319,12 @@
         <f t="shared" si="2"/>
         <v>102.45201830476057</v>
       </c>
-      <c r="P18" s="9">
+      <c r="P18" s="34">
         <f t="shared" ref="P18:P24" si="3">SUM(K18:O18)</f>
         <v>303.80438494638338</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +5362,7 @@
         <v>51.226009152380286</v>
       </c>
       <c r="N19" s="9">
-        <f t="shared" si="4"/>
+        <f>N18/((1+$C$19)^(N15-$K$15))</f>
         <v>70.559241256722132</v>
       </c>
       <c r="O19" s="9">
@@ -5003,8 +5373,11 @@
         <f t="shared" si="3"/>
         <v>233.08367149014916</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
@@ -5049,12 +5422,12 @@
         <f t="shared" si="5"/>
         <v>515.78887515194117</v>
       </c>
-      <c r="P20" s="9">
+      <c r="P20" s="34">
         <f t="shared" si="3"/>
         <v>-743.88592120016904</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -5099,12 +5472,12 @@
         <f t="shared" si="6"/>
         <v>301.0682277054272</v>
       </c>
-      <c r="P21" s="9">
+      <c r="P21" s="34">
         <f t="shared" si="3"/>
         <v>-474.95676848417799</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -5149,12 +5522,12 @@
         <f t="shared" si="7"/>
         <v>113.5475381714249</v>
       </c>
-      <c r="P22" s="9">
+      <c r="P22" s="34">
         <f t="shared" si="3"/>
         <v>-2554.8179099020208</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
@@ -5199,12 +5572,12 @@
         <f t="shared" si="8"/>
         <v>571.7532455930334</v>
       </c>
-      <c r="P23" s="9">
+      <c r="P23" s="34">
         <f t="shared" si="3"/>
         <v>236.70763040440863</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
@@ -5249,7 +5622,7 @@
         <f t="shared" si="9"/>
         <v>350.12779664577562</v>
       </c>
-      <c r="P24" s="9">
+      <c r="P24" s="34">
         <f t="shared" si="3"/>
         <v>-259.11207590770658</v>
       </c>
@@ -5262,17 +5635,17 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3C1205-B505-47CC-9F42-6948E774DB05}">
-  <dimension ref="B6:AR12"/>
+  <dimension ref="B6:AR16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5564,10 +5937,111 @@
         <f>AR8/((1+B8)^(40))</f>
         <v>50737.65494327456</v>
       </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f>X7/((1+$B$8)^(X6-$W$6))</f>
+        <v>9523.8095238095229</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ref="Y9:AQ9" si="1">Y7/((1+$B$8)^(Y6-$W$6))</f>
+        <v>9070.2947845804993</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>8638.3759853147603</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="1"/>
+        <v>8227.0247479188201</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="1"/>
+        <v>7835.2616646845891</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="1"/>
+        <v>7462.153966366277</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="1"/>
+        <v>7106.8133013012148</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="1"/>
+        <v>6768.3936202868717</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="1"/>
+        <v>6446.0891621779729</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="1"/>
+        <v>6139.1325354075934</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="1"/>
+        <v>5846.7928908643744</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="1"/>
+        <v>5568.3741817755954</v>
+      </c>
+      <c r="AJ9">
+        <f t="shared" si="1"/>
+        <v>5303.2135064529466</v>
+      </c>
+      <c r="AK9">
+        <f t="shared" si="1"/>
+        <v>5050.6795299551886</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="1"/>
+        <v>4810.1709809097019</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="1"/>
+        <v>4581.1152199140024</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="1"/>
+        <v>4362.9668761085732</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="1"/>
+        <v>4155.2065486748315</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="1"/>
+        <v>3957.3395701665063</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="1"/>
+        <v>3768.8948287300059</v>
+      </c>
+      <c r="AR9">
+        <f>SUM(W9:AQ9)</f>
+        <v>124622.10342539985</v>
+      </c>
     </row>
     <row r="12" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <f>AR9/((1+B8)^(20))</f>
+        <v>46968.760114544544</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5578,20 +6052,26 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4899B06-D786-4CEC-8B8A-040F849CA034}">
-  <dimension ref="A7:DN19"/>
+  <dimension ref="A5:DN46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView topLeftCell="AB19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL44" sqref="AL44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="45" max="45" width="14" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="1:118" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="7" spans="1:118" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:118" x14ac:dyDescent="0.25">
@@ -5991,7 +6471,7 @@
         <f t="shared" si="0"/>
         <v>10792.142736644701</v>
       </c>
-      <c r="M9" s="38">
+      <c r="M9" s="33">
         <f t="shared" si="0"/>
         <v>10792.142736644701</v>
       </c>
@@ -6782,15 +7262,15 @@
     </row>
     <row r="11" spans="1:118" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:118" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M12">
         <f>SUM(C10:M10)</f>
@@ -7219,22 +7699,22 @@
     </row>
     <row r="13" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M13">
         <f>SUM(N10:DN10)</f>
         <v>199990.98847993463</v>
       </c>
       <c r="N13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="2">
         <v>10792.142736644701</v>
@@ -7242,7 +7722,7 @@
     </row>
     <row r="16" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16">
         <f>$B$17</f>
@@ -7289,9 +7769,9 @@
         <v>10294.278788325608</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2">
         <v>10294.278788325608</v>
@@ -7341,21 +7821,724 @@
         <v>10294.278788325608</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M18">
         <f>SUM(C17:M17)</f>
         <v>190765.00000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M19">
         <v>190765</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>111</v>
+      </c>
+      <c r="R24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="39" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39">
+        <v>300000</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39">
+        <f>C39*D39</f>
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="AC40">
+        <v>25</v>
+      </c>
+      <c r="AD40">
+        <v>26</v>
+      </c>
+      <c r="AE40">
+        <v>27</v>
+      </c>
+      <c r="AF40">
+        <v>28</v>
+      </c>
+      <c r="AG40">
+        <v>29</v>
+      </c>
+      <c r="AH40">
+        <v>30</v>
+      </c>
+      <c r="AI40">
+        <v>31</v>
+      </c>
+      <c r="AJ40">
+        <v>32</v>
+      </c>
+      <c r="AK40">
+        <v>33</v>
+      </c>
+      <c r="AL40">
+        <v>34</v>
+      </c>
+      <c r="AM40">
+        <v>35</v>
+      </c>
+      <c r="AN40">
+        <v>36</v>
+      </c>
+      <c r="AO40">
+        <v>37</v>
+      </c>
+      <c r="AP40">
+        <v>38</v>
+      </c>
+      <c r="AQ40">
+        <v>39</v>
+      </c>
+      <c r="AR40">
+        <v>40</v>
+      </c>
+      <c r="AS40" s="17">
+        <v>41</v>
+      </c>
+      <c r="AT40">
+        <v>42</v>
+      </c>
+      <c r="AU40">
+        <v>43</v>
+      </c>
+      <c r="AV40">
+        <v>44</v>
+      </c>
+      <c r="AW40">
+        <v>45</v>
+      </c>
+      <c r="AX40">
+        <v>46</v>
+      </c>
+      <c r="AY40">
+        <v>47</v>
+      </c>
+      <c r="AZ40">
+        <v>48</v>
+      </c>
+      <c r="BA40">
+        <v>49</v>
+      </c>
+      <c r="BB40">
+        <v>50</v>
+      </c>
+      <c r="BC40">
+        <v>51</v>
+      </c>
+      <c r="BD40">
+        <v>52</v>
+      </c>
+      <c r="BE40">
+        <v>53</v>
+      </c>
+      <c r="BF40">
+        <v>54</v>
+      </c>
+      <c r="BG40">
+        <v>55</v>
+      </c>
+      <c r="BH40">
+        <v>56</v>
+      </c>
+      <c r="BI40">
+        <v>57</v>
+      </c>
+      <c r="BJ40">
+        <v>58</v>
+      </c>
+      <c r="BK40">
+        <v>59</v>
+      </c>
+      <c r="BL40">
+        <v>60</v>
+      </c>
+      <c r="BM40">
+        <v>61</v>
+      </c>
+      <c r="BN40">
+        <v>62</v>
+      </c>
+      <c r="BO40">
+        <v>63</v>
+      </c>
+      <c r="BP40">
+        <v>64</v>
+      </c>
+      <c r="BQ40">
+        <v>65</v>
+      </c>
+      <c r="BR40">
+        <v>66</v>
+      </c>
+      <c r="BS40">
+        <v>67</v>
+      </c>
+      <c r="BT40">
+        <v>68</v>
+      </c>
+      <c r="BU40">
+        <v>69</v>
+      </c>
+      <c r="BV40">
+        <v>70</v>
+      </c>
+      <c r="BW40">
+        <v>71</v>
+      </c>
+      <c r="BX40">
+        <v>72</v>
+      </c>
+      <c r="BY40">
+        <v>73</v>
+      </c>
+      <c r="BZ40">
+        <v>74</v>
+      </c>
+      <c r="CA40">
+        <v>75</v>
+      </c>
+      <c r="CB40">
+        <v>76</v>
+      </c>
+      <c r="CC40">
+        <v>77</v>
+      </c>
+      <c r="CD40">
+        <v>78</v>
+      </c>
+      <c r="CE40">
+        <v>79</v>
+      </c>
+      <c r="CF40">
+        <v>80</v>
+      </c>
+      <c r="CG40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41">
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AC41">
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" ref="F41:AR41" si="106">$C$41</f>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AJ41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AK41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AL41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AM41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AO41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AP41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AQ41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AR41">
+        <f t="shared" si="106"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AS41" s="17">
+        <f>$E$39</f>
+        <v>3600000</v>
+      </c>
+      <c r="AT41" s="17">
+        <f t="shared" ref="AT41:CF41" si="107">$E$39</f>
+        <v>3600000</v>
+      </c>
+      <c r="AU41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="AV41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="AW41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="AX41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="AY41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="AZ41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BA41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BB41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BC41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BD41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BE41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BF41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BG41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BH41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BI41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BJ41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BK41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BL41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BM41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BN41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BO41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BP41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BQ41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BR41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BS41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BT41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BU41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BV41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BW41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BX41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BY41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="BZ41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CA41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CB41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CC41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CD41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CE41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+      <c r="CF41" s="17">
+        <f t="shared" si="107"/>
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="AC42">
+        <f>AC41*(1+$C$38)^(40-AC40)</f>
+        <v>0</v>
+      </c>
+      <c r="AD42">
+        <f>AD41*(1+$C$38)^(40-AD40)</f>
+        <v>3763614.8180515277</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" ref="AE42:AR42" si="108">AE41*(1+$C$38)^(40-AE40)</f>
+        <v>3330632.5823464859</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="108"/>
+        <v>2947462.4622535273</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="108"/>
+        <v>2608373.8604013519</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="108"/>
+        <v>2308295.4516826128</v>
+      </c>
+      <c r="AI42">
+        <f t="shared" si="108"/>
+        <v>2042739.3377722239</v>
+      </c>
+      <c r="AJ42">
+        <f t="shared" si="108"/>
+        <v>1807733.9272320566</v>
+      </c>
+      <c r="AK42">
+        <f t="shared" si="108"/>
+        <v>1599764.5373735016</v>
+      </c>
+      <c r="AL42">
+        <f t="shared" si="108"/>
+        <v>1415720.8295340722</v>
+      </c>
+      <c r="AM42">
+        <f t="shared" si="108"/>
+        <v>1252850.2916230729</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="108"/>
+        <v>1108717.0722328082</v>
+      </c>
+      <c r="AO42">
+        <f t="shared" si="108"/>
+        <v>981165.55064850289</v>
+      </c>
+      <c r="AP42">
+        <f t="shared" si="108"/>
+        <v>868288.09791902918</v>
+      </c>
+      <c r="AQ42">
+        <f t="shared" si="108"/>
+        <v>768396.54683099943</v>
+      </c>
+      <c r="AR42">
+        <f t="shared" si="108"/>
+        <v>679996.94409822964</v>
+      </c>
+      <c r="AS42" s="17">
+        <f>AS41/(1+$C$38)^(AS40-$AR$40)</f>
+        <v>3185840.7079646019</v>
+      </c>
+      <c r="AT42">
+        <f>AT41/(1+$C$38)^(AT40-$AR$40)</f>
+        <v>2819328.0601456659</v>
+      </c>
+      <c r="AU42">
+        <f t="shared" ref="AT42:CF42" si="109">AU41/(1+$C$38)^(AU40-$AR$40)</f>
+        <v>2494980.5841997047</v>
+      </c>
+      <c r="AV42">
+        <f t="shared" si="109"/>
+        <v>2207947.4196457565</v>
+      </c>
+      <c r="AW42">
+        <f t="shared" si="109"/>
+        <v>1953935.7695980149</v>
+      </c>
+      <c r="AX42">
+        <f t="shared" si="109"/>
+        <v>1729146.6987593055</v>
+      </c>
+      <c r="AY42">
+        <f t="shared" si="109"/>
+        <v>1530218.3174861113</v>
+      </c>
+      <c r="AZ42">
+        <f t="shared" si="109"/>
+        <v>1354175.5022000985</v>
+      </c>
+      <c r="BA42">
+        <f t="shared" si="109"/>
+        <v>1198385.4001770783</v>
+      </c>
+      <c r="BB42">
+        <f t="shared" si="109"/>
+        <v>1060518.0532540518</v>
+      </c>
+      <c r="BC42">
+        <f t="shared" si="109"/>
+        <v>938511.55155225843</v>
+      </c>
+      <c r="BD42">
+        <f t="shared" si="109"/>
+        <v>830541.19606394565</v>
+      </c>
+      <c r="BE42">
+        <f t="shared" si="109"/>
+        <v>734992.20890614658</v>
+      </c>
+      <c r="BF42">
+        <f t="shared" si="109"/>
+        <v>650435.58310278482</v>
+      </c>
+      <c r="BG42">
+        <f t="shared" si="109"/>
+        <v>575606.710710429</v>
+      </c>
+      <c r="BH42">
+        <f t="shared" si="109"/>
+        <v>509386.46965524694</v>
+      </c>
+      <c r="BI42">
+        <f t="shared" si="109"/>
+        <v>450784.48642057256</v>
+      </c>
+      <c r="BJ42">
+        <f t="shared" si="109"/>
+        <v>398924.32426599349</v>
+      </c>
+      <c r="BK42">
+        <f t="shared" si="109"/>
+        <v>353030.37545663147</v>
+      </c>
+      <c r="BL42">
+        <f t="shared" si="109"/>
+        <v>312416.26146604557</v>
+      </c>
+      <c r="BM42">
+        <f t="shared" si="109"/>
+        <v>276474.56766906689</v>
+      </c>
+      <c r="BN42">
+        <f t="shared" si="109"/>
+        <v>244667.75899917429</v>
+      </c>
+      <c r="BO42">
+        <f t="shared" si="109"/>
+        <v>216520.14070723389</v>
+      </c>
+      <c r="BP42">
+        <f t="shared" si="109"/>
+        <v>191610.74398870257</v>
+      </c>
+      <c r="BQ42">
+        <f t="shared" si="109"/>
+        <v>169567.03007849786</v>
+      </c>
+      <c r="BR42">
+        <f t="shared" si="109"/>
+        <v>150059.31865353795</v>
+      </c>
+      <c r="BS42">
+        <f t="shared" si="109"/>
+        <v>132795.85721552034</v>
+      </c>
+      <c r="BT42">
+        <f t="shared" si="109"/>
+        <v>117518.45771284986</v>
+      </c>
+      <c r="BU42">
+        <f t="shared" si="109"/>
+        <v>103998.63514411492</v>
+      </c>
+      <c r="BV42">
+        <f t="shared" si="109"/>
+        <v>92034.190393022087</v>
+      </c>
+      <c r="BW42">
+        <f t="shared" si="109"/>
+        <v>81446.186188515116</v>
+      </c>
+      <c r="BX42">
+        <f t="shared" si="109"/>
+        <v>72076.270963287723</v>
+      </c>
+      <c r="BY42">
+        <f t="shared" si="109"/>
+        <v>63784.310586980297</v>
+      </c>
+      <c r="BZ42">
+        <f t="shared" si="109"/>
+        <v>56446.292554849824</v>
+      </c>
+      <c r="CA42">
+        <f t="shared" si="109"/>
+        <v>49952.471287477725</v>
+      </c>
+      <c r="CB42">
+        <f t="shared" si="109"/>
+        <v>44205.726803077639</v>
+      </c>
+      <c r="CC42">
+        <f t="shared" si="109"/>
+        <v>39120.11221511296</v>
+      </c>
+      <c r="CD42">
+        <f t="shared" si="109"/>
+        <v>34619.568331958377</v>
+      </c>
+      <c r="CE42">
+        <f t="shared" si="109"/>
+        <v>30636.786134476442</v>
+      </c>
+      <c r="CF42">
+        <f t="shared" si="109"/>
+        <v>27112.200119005702</v>
+      </c>
+      <c r="CG42">
+        <f>SUM(AS42:CF42)</f>
+        <v>27483752.306776911</v>
+      </c>
+    </row>
+    <row r="45" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="AR45" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS45" s="2">
+        <f>SUM(AS42:CF42)</f>
+        <v>27483752.306776911</v>
+      </c>
+    </row>
+    <row r="46" spans="2:85" x14ac:dyDescent="0.25">
+      <c r="AR46" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS46">
+        <f>SUM(AD42:AR42)</f>
+        <v>27483752.310000006</v>
       </c>
     </row>
   </sheetData>
@@ -7369,7 +8552,7 @@
   <dimension ref="A8:L13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:L8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7380,42 +8563,42 @@
   <sheetData>
     <row r="8" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>1000</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="H8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="36" t="s">
+      <c r="J8" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="36" t="s">
+      <c r="K8" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="L8" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -7599,7 +8782,7 @@
   <dimension ref="B6:M12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:L6"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7610,39 +8793,39 @@
   <sheetData>
     <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>10000</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="G6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="36" t="s">
+      <c r="I6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="J6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="K6" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="L6" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -7671,7 +8854,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1">
         <v>0.15</v>
@@ -7842,7 +9025,7 @@
         <v>-6.3664629124104977E-12</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -7856,7 +9039,7 @@
   <dimension ref="A6:K12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:K6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7867,29 +9050,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="F6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="36" t="s">
+      <c r="H6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="I6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="J6" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="K6" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -7921,7 +9104,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>10000</v>
@@ -7960,7 +9143,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -7999,7 +9182,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1">
         <v>0.15</v>
@@ -8117,10 +9300,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0947BD5-E75E-478F-9753-E3E7B8E955A0}">
-  <dimension ref="A3:L11"/>
+  <dimension ref="A3:L15"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8131,44 +9314,44 @@
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>10000</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="F5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="36" t="s">
+      <c r="H5" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="I5" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="J5" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="K5" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="K5" s="36" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -8200,7 +9383,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
         <v>0.12</v>
@@ -8220,7 +9403,7 @@
         <f>E7*F7</f>
         <v>1200</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="32">
         <v>1200</v>
       </c>
       <c r="I7">
@@ -8309,7 +9492,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -8372,6 +9555,50 @@
       <c r="K11" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>10000</v>
+      </c>
+      <c r="F14">
+        <v>1200</v>
+      </c>
+      <c r="J14">
+        <v>11200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f>J14</f>
+        <v>11200</v>
+      </c>
+      <c r="F15">
+        <f>E15*F7</f>
+        <v>1344</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>1344</v>
+      </c>
+      <c r="H15" s="2">
+        <f>J14/4</f>
+        <v>2800</v>
+      </c>
+      <c r="I15">
+        <f>G15+H15</f>
+        <v>4144</v>
       </c>
     </row>
   </sheetData>
@@ -8397,7 +9624,7 @@
   <sheetData>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -8414,7 +9641,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -8433,7 +9660,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1">
         <v>0.18</v>
@@ -8448,7 +9675,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>0.06</v>
@@ -8462,9 +9689,9 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="34">
+        <v>59</v>
+      </c>
+      <c r="D14" s="29">
         <f>((1+D12)/(1+D13))-1</f>
         <v>0.1132075471698113</v>
       </c>
@@ -8478,7 +9705,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -8512,18 +9739,18 @@
   <sheetData>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
         <v>0.1</v>
@@ -8531,7 +9758,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <f>B7/12</f>
@@ -8543,7 +9770,7 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="28">
         <v>8.3332999999999996E-5</v>
       </c>
       <c r="D9">
@@ -8834,7 +10061,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>88.218924213350277</v>
@@ -8847,7 +10074,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <f>SUM(D11:AB11)</f>
@@ -8856,7 +10083,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16">
         <f>B6*(1+B8)^(24)</f>
@@ -8898,9 +10125,9 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="33">
+        <v>54</v>
+      </c>
+      <c r="B7" s="28">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="C7" s="2">
@@ -8977,7 +10204,7 @@
   <sheetData>
     <row r="7" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>2000</v>
@@ -9009,7 +10236,7 @@
     </row>
     <row r="8" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>0.04</v>
@@ -9041,7 +10268,7 @@
     </row>
     <row r="9" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <f>B8/12</f>
@@ -9051,7 +10278,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:76" x14ac:dyDescent="0.25">
@@ -9059,15 +10286,15 @@
         <v>5000</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -9290,7 +10517,7 @@
       </c>
     </row>
     <row r="13" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
+      <c r="A13" s="28">
         <v>3.3E-3</v>
       </c>
       <c r="B13">
@@ -9891,7 +11118,7 @@
     </row>
     <row r="16" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16">
         <v>29.913456439437823</v>
@@ -9902,7 +11129,7 @@
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17">
         <f>SUM(D14:BX14)</f>
@@ -9911,7 +11138,7 @@
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18">
         <f>5000-B7*(1+A13)^(B13)</f>
@@ -9926,20 +11153,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52B2D2D-79F0-4C69-B426-D991CA3BA68C}">
-  <dimension ref="B7:O19"/>
+  <dimension ref="B3:O19"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="B4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O7">
         <f>O11/((1+5%)^(3))</f>
         <v>369.7070665000694</v>
       </c>
     </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>14</v>
@@ -10023,7 +11260,7 @@
         <f t="shared" si="0"/>
         <v>142.85714285714286</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="2">
         <f>SUM(J11:N11)</f>
         <v>427.98214285714289</v>
       </c>
@@ -10070,7 +11307,7 @@
         <f>H12*(1+$C$12)^($M$10-N10)</f>
         <v>39.130434782608702</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="2">
         <f>SUM(J12:N12)</f>
         <v>108.8054347826087</v>
       </c>
@@ -10117,7 +11354,7 @@
         <f>H13*(1+$C$13)^($M$10-N10)</f>
         <v>136.36363636363635</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="2">
         <f>SUM(J13:N13)</f>
         <v>404.36363636363637</v>
       </c>
@@ -10164,7 +11401,7 @@
         <f t="shared" si="3"/>
         <v>45.454545454545453</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="2">
         <f t="shared" ref="O14:O19" si="4">SUM(J14:N14)</f>
         <v>439.45454545454544</v>
       </c>
@@ -10211,7 +11448,7 @@
         <f t="shared" si="5"/>
         <v>847.45762711864415</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="2">
         <f t="shared" si="4"/>
         <v>-1222.2283728813554</v>
       </c>
@@ -10258,7 +11495,7 @@
         <f t="shared" si="6"/>
         <v>740.74074074074065</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="2">
         <f t="shared" si="4"/>
         <v>-1168.5717592592598</v>
       </c>
@@ -10305,7 +11542,7 @@
         <f t="shared" si="7"/>
         <v>291.97080291970804</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="2">
         <f t="shared" si="4"/>
         <v>-6569.3386970802931</v>
       </c>
@@ -10352,7 +11589,7 @@
         <f t="shared" si="8"/>
         <v>869.56521739130449</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <f t="shared" si="4"/>
         <v>360.0027173913054</v>
       </c>
@@ -10399,7 +11636,7 @@
         <f t="shared" si="9"/>
         <v>769.23076923076917</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="2">
         <f t="shared" si="4"/>
         <v>-569.26923076923174</v>
       </c>
@@ -10422,7 +11659,7 @@
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -10518,7 +11755,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -10532,7 +11769,7 @@
   <dimension ref="A2:N14"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10543,8 +11780,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I2" t="s">
-        <v>17</v>
+      <c r="I2" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -10635,7 +11872,7 @@
         <f t="shared" si="0"/>
         <v>123.40537121878229</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="34">
         <f>SUM(I6:M6)</f>
         <v>369.7070665000694</v>
       </c>
@@ -10682,7 +11919,7 @@
         <f t="shared" si="1"/>
         <v>25.728896051686505</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="34">
         <f t="shared" ref="N7:N14" si="2">SUM(I7:M7)</f>
         <v>71.541339546385288</v>
       </c>
@@ -10729,7 +11966,7 @@
         <f t="shared" si="3"/>
         <v>102.45201830476056</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="34">
         <f t="shared" si="2"/>
         <v>303.80438494638332</v>
       </c>
@@ -10776,7 +12013,7 @@
         <f t="shared" si="4"/>
         <v>34.150672768253521</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="34">
         <f t="shared" si="2"/>
         <v>330.16870432347508</v>
       </c>
@@ -10823,7 +12060,7 @@
         <f t="shared" si="5"/>
         <v>515.78887515194117</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="34">
         <f t="shared" si="2"/>
         <v>-743.88592120016904</v>
       </c>
@@ -10870,7 +12107,7 @@
         <f t="shared" si="6"/>
         <v>301.0682277054272</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="34">
         <f t="shared" si="2"/>
         <v>-474.95676848417799</v>
       </c>
@@ -10917,7 +12154,7 @@
         <f t="shared" si="7"/>
         <v>113.54753817142492</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="34">
         <f t="shared" si="2"/>
         <v>-2554.8179099020208</v>
       </c>
@@ -10964,7 +12201,7 @@
         <f t="shared" si="8"/>
         <v>571.7532455930334</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="34">
         <f t="shared" si="2"/>
         <v>236.70763040440886</v>
       </c>
@@ -11011,7 +12248,7 @@
         <f t="shared" si="9"/>
         <v>350.12779664577562</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="34">
         <f t="shared" si="2"/>
         <v>-259.11207590770658</v>
       </c>
@@ -11027,7 +12264,7 @@
   <dimension ref="B9:L15"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11079,7 +12316,7 @@
         <v>0.1</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I10" s="9">
         <f>1/((1+C10)^(I9-$H$9))</f>
@@ -11114,21 +12351,21 @@
       <c r="F11" s="5">
         <v>0.2</v>
       </c>
-      <c r="I11" s="9">
-        <f>1/((1+C11)^(I10-$H$9))</f>
-        <v>0.88068407877936705</v>
-      </c>
-      <c r="J11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.89091546059484217</v>
-      </c>
-      <c r="K11" s="9">
-        <f t="shared" ref="K11:K15" si="1">1/((1+E11)^(K10-$H$9))</f>
-        <v>0.87198689474982538</v>
-      </c>
-      <c r="L11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.88291347190414204</v>
+      <c r="I11" s="34">
+        <f>1/((1+C11))</f>
+        <v>0.86956521739130443</v>
+      </c>
+      <c r="J11" s="34">
+        <f>1/((1+C11)*(1+D11))</f>
+        <v>0.7561436672967865</v>
+      </c>
+      <c r="K11" s="34">
+        <f>1/((1+E11)*(1+D11)*(1+C11))</f>
+        <v>0.63011972274732209</v>
+      </c>
+      <c r="L11" s="34">
+        <f>1/((1+F11)*(1+E11)*(1+D11)*(1+C11))</f>
+        <v>0.52509976895610178</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -11148,20 +12385,20 @@
         <v>0.15</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" ref="I12:I15" si="2">1/((1+C12)^(I11-$H$9))</f>
-        <v>0.82158574326292821</v>
+        <f t="shared" ref="I12:I15" si="1">1/((1+C12)^(I11-$H$9))</f>
+        <v>0.8236267123512192</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" si="0"/>
-        <v>0.85007296351916661</v>
+        <f>1/((1+D12)^(J11-$H$9))</f>
+        <v>0.87121952971932737</v>
       </c>
       <c r="K12" s="9">
-        <f t="shared" si="1"/>
-        <v>0.8852629299268614</v>
+        <f t="shared" ref="K12:K15" si="2">1/((1+E12)^(K11-$H$9))</f>
+        <v>0.91569974588265246</v>
       </c>
       <c r="L12" s="9">
         <f t="shared" si="0"/>
-        <v>0.88391205924727112</v>
+        <v>0.92923931940565763</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -11181,20 +12418,20 @@
         <v>0.16</v>
       </c>
       <c r="I13" s="9">
+        <f t="shared" si="1"/>
+        <v>0.91088326212660575</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.89212021870211344</v>
+      </c>
+      <c r="K13" s="9">
         <f t="shared" si="2"/>
-        <v>0.91109397410598703</v>
-      </c>
-      <c r="J13" s="9">
-        <f t="shared" si="0"/>
-        <v>0.89459553117535506</v>
-      </c>
-      <c r="K13" s="9">
-        <f t="shared" si="1"/>
-        <v>0.87687508727944996</v>
+        <v>0.87292279718988242</v>
       </c>
       <c r="L13" s="9">
         <f t="shared" si="0"/>
-        <v>0.87705091505723243</v>
+        <v>0.87117038216120479</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -11214,20 +12451,20 @@
         <v>0.15</v>
       </c>
       <c r="I14" s="9">
+        <f t="shared" si="1"/>
+        <v>0.89464705003874745</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.88277541436376639</v>
+      </c>
+      <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>0.89462401074105291</v>
-      </c>
-      <c r="J14" s="9">
-        <f t="shared" si="0"/>
-        <v>0.8824700670761757</v>
-      </c>
-      <c r="K14" s="9">
-        <f t="shared" si="1"/>
-        <v>0.88465833963889506</v>
+        <v>0.88514714197213495</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" si="0"/>
-        <v>0.88463660028388491</v>
+        <v>0.88536395958229064</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -11247,20 +12484,20 @@
         <v>0.4</v>
       </c>
       <c r="I15" s="9">
+        <f t="shared" si="1"/>
+        <v>0.7400600896039734</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.74302215373654135</v>
+      </c>
+      <c r="K15" s="9">
         <f t="shared" si="2"/>
-        <v>0.74006582663420883</v>
-      </c>
-      <c r="J15" s="9">
-        <f t="shared" si="0"/>
-        <v>0.74309849641173331</v>
-      </c>
-      <c r="K15" s="9">
-        <f t="shared" si="1"/>
-        <v>0.74255155959520081</v>
+        <v>0.74242944336004224</v>
       </c>
       <c r="L15" s="9">
         <f t="shared" si="0"/>
-        <v>0.74255699114908991</v>
+        <v>0.74237528280160858</v>
       </c>
     </row>
   </sheetData>
@@ -11271,15 +12508,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D673E0-9DCE-4121-9F76-3E19C7BD5D50}">
-  <dimension ref="B2:O20"/>
+  <dimension ref="B2:P20"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I2" s="10"/>
       <c r="J2" s="11">
         <v>0</v>
@@ -11297,9 +12534,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I3" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="15">
@@ -11314,10 +12551,13 @@
       <c r="N3" s="16">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4">
         <v>1250</v>
@@ -11332,7 +12572,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I5" s="22" t="s">
         <v>13</v>
       </c>
@@ -11353,12 +12593,12 @@
         <f>N4/((1+K3)*(1+L3)*(1+M3)*(1+N3))</f>
         <v>1054.0184453227932</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <f>SUM(K5:N5)</f>
         <v>4528.985507246377</v>
       </c>
     </row>
-    <row r="7" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I7" s="10"/>
       <c r="J7" s="11">
         <v>0</v>
@@ -11376,9 +12616,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I8" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="15">
@@ -11394,9 +12634,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I9" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9">
         <v>-4200</v>
@@ -11414,7 +12654,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I10" s="22" t="s">
         <v>13</v>
       </c>
@@ -11437,12 +12677,12 @@
         <f>N9/((1+N8)*(1+M8)*(1+L8)*(1+K8))</f>
         <v>1054.0184453227932</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="2">
         <f>SUM(J10:N10)</f>
         <v>-131.48880105401827</v>
       </c>
     </row>
-    <row r="12" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I12" s="10"/>
       <c r="J12" s="11">
         <v>0</v>
@@ -11460,9 +12700,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I13" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11478,9 +12718,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I14" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14">
         <v>-4200</v>
@@ -11498,7 +12738,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I15" s="22" t="s">
         <v>13</v>
       </c>
@@ -11521,14 +12761,14 @@
         <f>N14/((1+N13)*(1+M13)*(1+L13)*(1+K13))</f>
         <v>1227.5987775080332</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="2">
         <f>SUM(J15:N15)</f>
         <v>421.05007817348951</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="11">
@@ -11549,7 +12789,7 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I18" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="15">
@@ -11567,7 +12807,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I19" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19">
         <v>-3000</v>
@@ -11608,7 +12848,7 @@
         <f>N19/((1+N18)*(1+M18)*(1+L18)*(1+K18))</f>
         <v>571.65256590337424</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="2">
         <f>SUM(J20:N20)</f>
         <v>710.3518113219875</v>
       </c>
@@ -11624,14 +12864,14 @@
   <dimension ref="B8:H12"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -11672,7 +12912,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5">
@@ -11690,21 +12930,24 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="9">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
         <f>1/((1+D10)^(D8))</f>
         <v>0.86956521739130443</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="34">
         <f>1/((1+E10)^(E8))</f>
         <v>0.7561436672967865</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="34">
         <f t="shared" ref="F11:G11" si="0">1/((1+F10)^(F8))</f>
         <v>0.65751623243198831</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="34">
         <f t="shared" si="0"/>
         <v>0.57175324559303342</v>
       </c>
@@ -11713,23 +12956,23 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <f>D9*D11</f>
         <v>2173.913043478261</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f>E9*E11</f>
         <v>1890.3591682419662</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <f>F9*F11</f>
         <v>1643.7905810799707</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <f t="shared" ref="G12" si="1">G9*G11</f>
         <v>1429.3831139825836</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <f>SUM(D12:G12)</f>
         <v>7137.4459067827811</v>
       </c>
@@ -11745,14 +12988,14 @@
   <dimension ref="B7:H14"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -11795,7 +13038,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5">
@@ -11813,25 +13056,25 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
         <f>1/((1+0%)^(C7))</f>
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f>1/((1+D9)^(D7))</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f>1/((1+E9)^(E7))</f>
         <v>0.69444444444444442</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <f t="shared" ref="F10" si="0">1/((1+F9)^(F7))</f>
         <v>0.57870370370370372</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <f>1/((1+G9)^(G7))</f>
         <v>0.48225308641975312</v>
       </c>
@@ -11840,34 +13083,34 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <f>C8*C10</f>
         <v>10000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f t="shared" ref="D11:G11" si="1">D8*D10</f>
         <v>8333.3333333333339</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>6944.4444444444443</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>5787.0370370370374</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <f t="shared" si="1"/>
         <v>4822.5308641975316</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <f>SUM(C11:G11)</f>
         <v>35887.345679012345</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -11881,14 +13124,14 @@
   <dimension ref="B8:H11"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -11929,7 +13172,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5">
@@ -11949,23 +13192,23 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <f>D9/((1+D10)^(D8))</f>
         <v>2173.913043478261</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f>E9/((1+E10)^(E8))</f>
         <v>1890.3591682419662</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <f t="shared" ref="F11:G11" si="0">F9/((1+F10)^(F8))</f>
         <v>1643.7905810799709</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>1429.3831139825834</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <f>SUM(D11:G11)</f>
         <v>7137.445906782782</v>
       </c>

</xml_diff>

<commit_message>
exam practice and excel files
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week3/hw1.xlsx
+++ b/PM2/econ/week3/hw1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64650E43-3C1D-404F-90DD-CF7259844CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE55949-B1AD-47CF-801A-2DA3A1136054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="21" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="28" xr2:uid="{60FC90CF-4422-48E4-949B-85C13790FC61}"/>
   </bookViews>
   <sheets>
     <sheet name="ex1g" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="130">
   <si>
     <t>Flujos</t>
   </si>
@@ -431,6 +431,30 @@
   </si>
   <si>
     <t xml:space="preserve">despejando r: incremento de precio promedio por año </t>
+  </si>
+  <si>
+    <t>me prestan 2000 hoy y lo puedo pagar en 2 años, pero con intereses</t>
+  </si>
+  <si>
+    <t>en 2 años</t>
+  </si>
+  <si>
+    <t>suponiendo mensualidades vencidas</t>
+  </si>
+  <si>
+    <t>debo tener</t>
+  </si>
+  <si>
+    <t>suponiendo mensualidades anticipadas</t>
+  </si>
+  <si>
+    <t>2000 al f</t>
+  </si>
+  <si>
+    <t>se lleva a la 72 no al 71, ya que el 71 es la última anualidad, pero al final de tus pagos es el 72</t>
+  </si>
+  <si>
+    <t>se lleva al 72 - cell pq el 71 solo es hasta cuando pago, pero la meta la debo tener en el mes 72</t>
   </si>
 </sst>
 </file>
@@ -4460,7 +4484,7 @@
   <dimension ref="B6:K17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4785,7 +4809,7 @@
   <dimension ref="B6:L36"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8578,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F163BAD2-955A-4F03-BA07-1A966AD9705C}">
   <dimension ref="A8:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9753,10 +9777,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A782090-6A1E-43FD-AEE4-111472A01453}">
-  <dimension ref="A6:AB16"/>
+  <dimension ref="A6:AB25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10115,6 +10139,330 @@
       <c r="C16">
         <f>B6*(1+B8)^(24)</f>
         <v>2440.7819227511181</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2">
+        <v>88.149166790013567</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>7</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="N19">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <v>12</v>
+      </c>
+      <c r="P19">
+        <v>13</v>
+      </c>
+      <c r="Q19">
+        <v>14</v>
+      </c>
+      <c r="R19">
+        <v>15</v>
+      </c>
+      <c r="S19">
+        <v>16</v>
+      </c>
+      <c r="T19">
+        <v>17</v>
+      </c>
+      <c r="U19">
+        <v>18</v>
+      </c>
+      <c r="V19">
+        <v>19</v>
+      </c>
+      <c r="W19">
+        <v>20</v>
+      </c>
+      <c r="X19">
+        <v>21</v>
+      </c>
+      <c r="Y19">
+        <v>22</v>
+      </c>
+      <c r="Z19">
+        <v>23</v>
+      </c>
+      <c r="AA19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <f>$C$18</f>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:AA20" si="2">$C$18</f>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="2"/>
+        <v>88.149166790013567</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>C20*(1+$B$8)^(24-C19)</f>
+        <v>107.57644640331915</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:AA21" si="3">D20*(1+$B$8)^(24-D19)</f>
+        <v>106.68738486279587</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>105.80567093830996</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>104.93124390576192</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>104.0640435429044</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>103.20401012519446</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>102.35108442168047</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>101.50520769092276</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>100.6663216769482</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>99.834368605237898</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>99.009291178748327</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="3"/>
+        <v>98.191032573965273</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="3"/>
+        <v>97.379536436990378</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>96.57474687965987</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="3"/>
+        <v>95.776608475695753</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="3"/>
+        <v>94.985066256888345</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="3"/>
+        <v>94.200065709310763</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>93.421552769564386</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="3"/>
+        <v>92.649473821055608</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="3"/>
+        <v>91.883775690303068</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="3"/>
+        <v>91.124405643275779</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="3"/>
+        <v>90.371311381761117</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="3"/>
+        <v>89.624441039763099</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="3"/>
+        <v>88.883743179930349</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="3"/>
+        <v>88.149166790013567</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C21:AA21)</f>
+        <v>2438.8500000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <f>B25*(1+0.0083)^(24)</f>
+        <v>2438.8461706211951</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -10221,10 +10569,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3884B2-0C0A-4FC7-AD0F-165867150FEB}">
-  <dimension ref="A7:BX18"/>
+  <dimension ref="A7:BX36"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11154,7 +11502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>65</v>
       </c>
@@ -11163,12 +11511,1708 @@
         <v>2464.5899999999992</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>66</v>
       </c>
       <c r="E18">
         <f>5000-B7*(1+A13)^(B13)</f>
+        <v>2464.5883741592515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21">
+        <v>30.380912955443758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>13</v>
+      </c>
+      <c r="P22">
+        <v>14</v>
+      </c>
+      <c r="Q22">
+        <v>15</v>
+      </c>
+      <c r="R22">
+        <v>16</v>
+      </c>
+      <c r="S22">
+        <v>17</v>
+      </c>
+      <c r="T22">
+        <v>18</v>
+      </c>
+      <c r="U22">
+        <v>19</v>
+      </c>
+      <c r="V22">
+        <v>20</v>
+      </c>
+      <c r="W22">
+        <v>21</v>
+      </c>
+      <c r="X22">
+        <v>22</v>
+      </c>
+      <c r="Y22">
+        <v>23</v>
+      </c>
+      <c r="Z22">
+        <v>24</v>
+      </c>
+      <c r="AA22">
+        <v>25</v>
+      </c>
+      <c r="AB22">
+        <v>26</v>
+      </c>
+      <c r="AC22">
+        <v>27</v>
+      </c>
+      <c r="AD22">
+        <v>28</v>
+      </c>
+      <c r="AE22">
+        <v>29</v>
+      </c>
+      <c r="AF22">
+        <v>30</v>
+      </c>
+      <c r="AG22">
+        <v>31</v>
+      </c>
+      <c r="AH22">
+        <v>32</v>
+      </c>
+      <c r="AI22">
+        <v>33</v>
+      </c>
+      <c r="AJ22">
+        <v>34</v>
+      </c>
+      <c r="AK22">
+        <v>35</v>
+      </c>
+      <c r="AL22">
+        <v>36</v>
+      </c>
+      <c r="AM22">
+        <v>37</v>
+      </c>
+      <c r="AN22">
+        <v>38</v>
+      </c>
+      <c r="AO22">
+        <v>39</v>
+      </c>
+      <c r="AP22">
+        <v>40</v>
+      </c>
+      <c r="AQ22">
+        <v>41</v>
+      </c>
+      <c r="AR22">
+        <v>42</v>
+      </c>
+      <c r="AS22">
+        <v>43</v>
+      </c>
+      <c r="AT22">
+        <v>44</v>
+      </c>
+      <c r="AU22">
+        <v>45</v>
+      </c>
+      <c r="AV22">
+        <v>46</v>
+      </c>
+      <c r="AW22">
+        <v>47</v>
+      </c>
+      <c r="AX22">
+        <v>48</v>
+      </c>
+      <c r="AY22">
+        <v>49</v>
+      </c>
+      <c r="AZ22">
+        <v>50</v>
+      </c>
+      <c r="BA22">
+        <v>51</v>
+      </c>
+      <c r="BB22">
+        <v>52</v>
+      </c>
+      <c r="BC22">
+        <v>53</v>
+      </c>
+      <c r="BD22">
+        <v>54</v>
+      </c>
+      <c r="BE22">
+        <v>55</v>
+      </c>
+      <c r="BF22">
+        <v>56</v>
+      </c>
+      <c r="BG22">
+        <v>57</v>
+      </c>
+      <c r="BH22">
+        <v>58</v>
+      </c>
+      <c r="BI22">
+        <v>59</v>
+      </c>
+      <c r="BJ22">
+        <v>60</v>
+      </c>
+      <c r="BK22">
+        <v>61</v>
+      </c>
+      <c r="BL22">
+        <v>62</v>
+      </c>
+      <c r="BM22">
+        <v>63</v>
+      </c>
+      <c r="BN22">
+        <v>64</v>
+      </c>
+      <c r="BO22">
+        <v>65</v>
+      </c>
+      <c r="BP22">
+        <v>66</v>
+      </c>
+      <c r="BQ22">
+        <v>67</v>
+      </c>
+      <c r="BR22">
+        <v>68</v>
+      </c>
+      <c r="BS22">
+        <v>69</v>
+      </c>
+      <c r="BT22">
+        <v>70</v>
+      </c>
+      <c r="BU22">
+        <v>71</v>
+      </c>
+      <c r="BV22">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>2000</v>
+      </c>
+      <c r="C23">
+        <f>$C$21</f>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:BO23" si="4">$C$21</f>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AF23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AL23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AR23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AS23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AT23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AU23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AV23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AW23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AY23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="AZ23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BA23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BB23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BC23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BD23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BE23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BF23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BG23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BH23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BI23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BJ23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BK23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BL23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BM23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BN23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BO23">
+        <f t="shared" si="4"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BP23">
+        <f t="shared" ref="BP23:BV23" si="5">$C$21</f>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BQ23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BR23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BS23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BT23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BU23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+      <c r="BV23">
+        <f t="shared" si="5"/>
+        <v>30.380912955443758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:BN24" si="6">C23*(1+$A$13)^($BV$22-C22)</f>
+        <v>38.387381596176574</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>38.261119900504895</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>38.13527349796162</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="6"/>
+        <v>38.009841022587089</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>37.884821112914466</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="6"/>
+        <v>37.76021241195501</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>37.636013567183298</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>37.512223230522572</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>37.388840058330082</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>37.265862711382503</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="6"/>
+        <v>37.143289854861465</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="6"/>
+        <v>37.021120158338945</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
+        <v>36.899352295762924</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="6"/>
+        <v>36.777984945442959</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="6"/>
+        <v>36.657016790035833</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>36.536446516531278</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>36.416272816237701</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="6"/>
+        <v>36.296494384767961</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="6"/>
+        <v>36.177109922025274</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="6"/>
+        <v>36.058118132189044</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="6"/>
+        <v>35.939517723700831</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="6"/>
+        <v>35.821307409250302</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="6"/>
+        <v>35.703485905761283</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="6"/>
+        <v>35.586051934377835</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="6"/>
+        <v>35.469004220450351</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="6"/>
+        <v>35.35234149352172</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="6"/>
+        <v>35.236062487313589</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="6"/>
+        <v>35.120165939712535</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="6"/>
+        <v>35.004650592756434</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" si="6"/>
+        <v>34.889515192620784</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="6"/>
+        <v>34.774758489605077</v>
+      </c>
+      <c r="AH24">
+        <f t="shared" si="6"/>
+        <v>34.660379238119283</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" si="6"/>
+        <v>34.546376196670273</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" si="6"/>
+        <v>34.43274812784837</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" si="6"/>
+        <v>34.319493798313928</v>
+      </c>
+      <c r="AL24">
+        <f t="shared" si="6"/>
+        <v>34.20661197878394</v>
+      </c>
+      <c r="AM24">
+        <f t="shared" si="6"/>
+        <v>34.094101444018676</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="6"/>
+        <v>33.981960972808402</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="6"/>
+        <v>33.870189347960135</v>
+      </c>
+      <c r="AP24">
+        <f t="shared" si="6"/>
+        <v>33.758785356284392</v>
+      </c>
+      <c r="AQ24">
+        <f t="shared" si="6"/>
+        <v>33.647747788582073</v>
+      </c>
+      <c r="AR24">
+        <f t="shared" si="6"/>
+        <v>33.53707543963128</v>
+      </c>
+      <c r="AS24">
+        <f t="shared" si="6"/>
+        <v>33.426767108174303</v>
+      </c>
+      <c r="AT24">
+        <f t="shared" si="6"/>
+        <v>33.316821596904518</v>
+      </c>
+      <c r="AU24">
+        <f t="shared" si="6"/>
+        <v>33.20723771245342</v>
+      </c>
+      <c r="AV24">
+        <f t="shared" si="6"/>
+        <v>33.098014265377671</v>
+      </c>
+      <c r="AW24">
+        <f t="shared" si="6"/>
+        <v>32.989150070146181</v>
+      </c>
+      <c r="AX24">
+        <f t="shared" si="6"/>
+        <v>32.880643945127261</v>
+      </c>
+      <c r="AY24">
+        <f t="shared" si="6"/>
+        <v>32.772494712575757</v>
+      </c>
+      <c r="AZ24">
+        <f t="shared" si="6"/>
+        <v>32.664701198620307</v>
+      </c>
+      <c r="BA24">
+        <f t="shared" si="6"/>
+        <v>32.557262233250576</v>
+      </c>
+      <c r="BB24">
+        <f t="shared" si="6"/>
+        <v>32.45017665030457</v>
+      </c>
+      <c r="BC24">
+        <f t="shared" si="6"/>
+        <v>32.343443287455962</v>
+      </c>
+      <c r="BD24">
+        <f t="shared" si="6"/>
+        <v>32.237060986201492</v>
+      </c>
+      <c r="BE24">
+        <f t="shared" si="6"/>
+        <v>32.131028591848391</v>
+      </c>
+      <c r="BF24">
+        <f t="shared" si="6"/>
+        <v>32.025344953501836</v>
+      </c>
+      <c r="BG24">
+        <f t="shared" si="6"/>
+        <v>31.920008924052464</v>
+      </c>
+      <c r="BH24">
+        <f t="shared" si="6"/>
+        <v>31.815019360163916</v>
+      </c>
+      <c r="BI24">
+        <f t="shared" si="6"/>
+        <v>31.710375122260455</v>
+      </c>
+      <c r="BJ24">
+        <f t="shared" si="6"/>
+        <v>31.606075074514553</v>
+      </c>
+      <c r="BK24">
+        <f t="shared" si="6"/>
+        <v>31.502118084834599</v>
+      </c>
+      <c r="BL24">
+        <f t="shared" si="6"/>
+        <v>31.39850302485258</v>
+      </c>
+      <c r="BM24">
+        <f t="shared" si="6"/>
+        <v>31.295228769911869</v>
+      </c>
+      <c r="BN24">
+        <f t="shared" si="6"/>
+        <v>31.192294199054988</v>
+      </c>
+      <c r="BO24">
+        <f t="shared" ref="BO24:BV24" si="7">BO23*(1+$A$13)^($BV$22-BO22)</f>
+        <v>31.089698195011447</v>
+      </c>
+      <c r="BP24">
+        <f t="shared" si="7"/>
+        <v>30.987439644185631</v>
+      </c>
+      <c r="BQ24">
+        <f t="shared" si="7"/>
+        <v>30.885517436644701</v>
+      </c>
+      <c r="BR24">
+        <f t="shared" si="7"/>
+        <v>30.783930466106547</v>
+      </c>
+      <c r="BS24">
+        <f t="shared" si="7"/>
+        <v>30.682677629927781</v>
+      </c>
+      <c r="BT24">
+        <f t="shared" si="7"/>
+        <v>30.581757829091778</v>
+      </c>
+      <c r="BU24">
+        <f t="shared" si="7"/>
+        <v>30.481169968196724</v>
+      </c>
+      <c r="BV24">
+        <f t="shared" si="7"/>
+        <v>30.380912955443758</v>
+      </c>
+    </row>
+    <row r="25" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C24:BV24)</f>
+        <v>2464.5899999999988</v>
+      </c>
+    </row>
+    <row r="26" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26">
+        <f>5000-B23*(1+A13)^(72)</f>
+        <v>2464.5883741592515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29">
+        <v>30.280985702625099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>8</v>
+      </c>
+      <c r="K30">
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <v>10</v>
+      </c>
+      <c r="M30">
+        <v>11</v>
+      </c>
+      <c r="N30">
+        <v>12</v>
+      </c>
+      <c r="O30">
+        <v>13</v>
+      </c>
+      <c r="P30">
+        <v>14</v>
+      </c>
+      <c r="Q30">
+        <v>15</v>
+      </c>
+      <c r="R30">
+        <v>16</v>
+      </c>
+      <c r="S30">
+        <v>17</v>
+      </c>
+      <c r="T30">
+        <v>18</v>
+      </c>
+      <c r="U30">
+        <v>19</v>
+      </c>
+      <c r="V30">
+        <v>20</v>
+      </c>
+      <c r="W30">
+        <v>21</v>
+      </c>
+      <c r="X30">
+        <v>22</v>
+      </c>
+      <c r="Y30">
+        <v>23</v>
+      </c>
+      <c r="Z30">
+        <v>24</v>
+      </c>
+      <c r="AA30">
+        <v>25</v>
+      </c>
+      <c r="AB30">
+        <v>26</v>
+      </c>
+      <c r="AC30">
+        <v>27</v>
+      </c>
+      <c r="AD30">
+        <v>28</v>
+      </c>
+      <c r="AE30">
+        <v>29</v>
+      </c>
+      <c r="AF30">
+        <v>30</v>
+      </c>
+      <c r="AG30">
+        <v>31</v>
+      </c>
+      <c r="AH30">
+        <v>32</v>
+      </c>
+      <c r="AI30">
+        <v>33</v>
+      </c>
+      <c r="AJ30">
+        <v>34</v>
+      </c>
+      <c r="AK30">
+        <v>35</v>
+      </c>
+      <c r="AL30">
+        <v>36</v>
+      </c>
+      <c r="AM30">
+        <v>37</v>
+      </c>
+      <c r="AN30">
+        <v>38</v>
+      </c>
+      <c r="AO30">
+        <v>39</v>
+      </c>
+      <c r="AP30">
+        <v>40</v>
+      </c>
+      <c r="AQ30">
+        <v>41</v>
+      </c>
+      <c r="AR30">
+        <v>42</v>
+      </c>
+      <c r="AS30">
+        <v>43</v>
+      </c>
+      <c r="AT30">
+        <v>44</v>
+      </c>
+      <c r="AU30">
+        <v>45</v>
+      </c>
+      <c r="AV30">
+        <v>46</v>
+      </c>
+      <c r="AW30">
+        <v>47</v>
+      </c>
+      <c r="AX30">
+        <v>48</v>
+      </c>
+      <c r="AY30">
+        <v>49</v>
+      </c>
+      <c r="AZ30">
+        <v>50</v>
+      </c>
+      <c r="BA30">
+        <v>51</v>
+      </c>
+      <c r="BB30">
+        <v>52</v>
+      </c>
+      <c r="BC30">
+        <v>53</v>
+      </c>
+      <c r="BD30">
+        <v>54</v>
+      </c>
+      <c r="BE30">
+        <v>55</v>
+      </c>
+      <c r="BF30">
+        <v>56</v>
+      </c>
+      <c r="BG30">
+        <v>57</v>
+      </c>
+      <c r="BH30">
+        <v>58</v>
+      </c>
+      <c r="BI30">
+        <v>59</v>
+      </c>
+      <c r="BJ30">
+        <v>60</v>
+      </c>
+      <c r="BK30">
+        <v>61</v>
+      </c>
+      <c r="BL30">
+        <v>62</v>
+      </c>
+      <c r="BM30">
+        <v>63</v>
+      </c>
+      <c r="BN30">
+        <v>64</v>
+      </c>
+      <c r="BO30">
+        <v>65</v>
+      </c>
+      <c r="BP30">
+        <v>66</v>
+      </c>
+      <c r="BQ30">
+        <v>67</v>
+      </c>
+      <c r="BR30">
+        <v>68</v>
+      </c>
+      <c r="BS30">
+        <v>69</v>
+      </c>
+      <c r="BT30">
+        <v>70</v>
+      </c>
+      <c r="BU30">
+        <v>71</v>
+      </c>
+      <c r="BV30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <f>$C$29</f>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="C31">
+        <f>$C$29</f>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:BO31" si="8">$C$29</f>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AI31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AJ31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AK31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AL31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AM31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AO31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AQ31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AR31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AS31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AT31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AU31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AV31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AW31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AX31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AY31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="AZ31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BA31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BB31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BC31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BD31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BE31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BF31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BG31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BH31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BI31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BJ31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BK31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BL31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BM31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BN31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BO31">
+        <f t="shared" si="8"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BP31">
+        <f t="shared" ref="BP31:BU31" si="9">$C$29</f>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BQ31">
+        <f t="shared" si="9"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BR31">
+        <f t="shared" si="9"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BS31">
+        <f t="shared" si="9"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BT31">
+        <f t="shared" si="9"/>
+        <v>30.280985702625099</v>
+      </c>
+      <c r="BU31">
+        <f t="shared" si="9"/>
+        <v>30.280985702625099</v>
+      </c>
+    </row>
+    <row r="32" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f>B31*(1+$A$13)^($BV$30-B30)</f>
+        <v>38.387381596176581</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:BN32" si="10">C31*(1+$A$13)^($BV$30-C30)</f>
+        <v>38.261119900504916</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="10"/>
+        <v>38.135273497961627</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="10"/>
+        <v>38.009841022587089</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="10"/>
+        <v>37.884821112914473</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="10"/>
+        <v>37.760212411955017</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>37.636013567183305</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="10"/>
+        <v>37.512223230522579</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="10"/>
+        <v>37.388840058330089</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="10"/>
+        <v>37.265862711382525</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="10"/>
+        <v>37.143289854861465</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="10"/>
+        <v>37.021120158338952</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="10"/>
+        <v>36.899352295762931</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="10"/>
+        <v>36.777984945442967</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="10"/>
+        <v>36.657016790035847</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="10"/>
+        <v>36.536446516531285</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="10"/>
+        <v>36.416272816237701</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="10"/>
+        <v>36.296494384767968</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="10"/>
+        <v>36.177109922025281</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="10"/>
+        <v>36.058118132189051</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="10"/>
+        <v>35.939517723700838</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="10"/>
+        <v>35.821307409250309</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="10"/>
+        <v>35.703485905761291</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="10"/>
+        <v>35.586051934377835</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="10"/>
+        <v>35.469004220450351</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="10"/>
+        <v>35.352341493521735</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="10"/>
+        <v>35.236062487313589</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="10"/>
+        <v>35.120165939712535</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="10"/>
+        <v>35.004650592756441</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="10"/>
+        <v>34.889515192620792</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="10"/>
+        <v>34.774758489605091</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="10"/>
+        <v>34.66037923811929</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="10"/>
+        <v>34.54637619667028</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="10"/>
+        <v>34.432748127848377</v>
+      </c>
+      <c r="AJ32">
+        <f t="shared" si="10"/>
+        <v>34.319493798313935</v>
+      </c>
+      <c r="AK32">
+        <f t="shared" si="10"/>
+        <v>34.20661197878394</v>
+      </c>
+      <c r="AL32">
+        <f t="shared" si="10"/>
+        <v>34.094101444018683</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="10"/>
+        <v>33.981960972808416</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="10"/>
+        <v>33.870189347960135</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="10"/>
+        <v>33.758785356284399</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="10"/>
+        <v>33.647747788582073</v>
+      </c>
+      <c r="AQ32">
+        <f t="shared" si="10"/>
+        <v>33.537075439631288</v>
+      </c>
+      <c r="AR32">
+        <f t="shared" si="10"/>
+        <v>33.426767108174303</v>
+      </c>
+      <c r="AS32">
+        <f t="shared" si="10"/>
+        <v>33.316821596904525</v>
+      </c>
+      <c r="AT32">
+        <f t="shared" si="10"/>
+        <v>33.207237712453427</v>
+      </c>
+      <c r="AU32">
+        <f t="shared" si="10"/>
+        <v>33.098014265377678</v>
+      </c>
+      <c r="AV32">
+        <f t="shared" si="10"/>
+        <v>32.989150070146188</v>
+      </c>
+      <c r="AW32">
+        <f t="shared" si="10"/>
+        <v>32.880643945127268</v>
+      </c>
+      <c r="AX32">
+        <f t="shared" si="10"/>
+        <v>32.772494712575764</v>
+      </c>
+      <c r="AY32">
+        <f t="shared" si="10"/>
+        <v>32.664701198620314</v>
+      </c>
+      <c r="AZ32">
+        <f t="shared" si="10"/>
+        <v>32.557262233250583</v>
+      </c>
+      <c r="BA32">
+        <f t="shared" si="10"/>
+        <v>32.450176650304577</v>
+      </c>
+      <c r="BB32">
+        <f t="shared" si="10"/>
+        <v>32.343443287455969</v>
+      </c>
+      <c r="BC32">
+        <f t="shared" si="10"/>
+        <v>32.237060986201506</v>
+      </c>
+      <c r="BD32">
+        <f t="shared" si="10"/>
+        <v>32.131028591848398</v>
+      </c>
+      <c r="BE32">
+        <f t="shared" si="10"/>
+        <v>32.025344953501836</v>
+      </c>
+      <c r="BF32">
+        <f t="shared" si="10"/>
+        <v>31.920008924052464</v>
+      </c>
+      <c r="BG32">
+        <f t="shared" si="10"/>
+        <v>31.815019360163927</v>
+      </c>
+      <c r="BH32">
+        <f t="shared" si="10"/>
+        <v>31.710375122260459</v>
+      </c>
+      <c r="BI32">
+        <f t="shared" si="10"/>
+        <v>31.60607507451456</v>
+      </c>
+      <c r="BJ32">
+        <f t="shared" si="10"/>
+        <v>31.502118084834603</v>
+      </c>
+      <c r="BK32">
+        <f t="shared" si="10"/>
+        <v>31.398503024852591</v>
+      </c>
+      <c r="BL32">
+        <f t="shared" si="10"/>
+        <v>31.295228769911876</v>
+      </c>
+      <c r="BM32">
+        <f t="shared" si="10"/>
+        <v>31.192294199054988</v>
+      </c>
+      <c r="BN32">
+        <f t="shared" si="10"/>
+        <v>31.089698195011451</v>
+      </c>
+      <c r="BO32">
+        <f t="shared" ref="BO32:BU32" si="11">BO31*(1+$A$13)^($BV$30-BO30)</f>
+        <v>30.987439644185638</v>
+      </c>
+      <c r="BP32">
+        <f t="shared" si="11"/>
+        <v>30.885517436644705</v>
+      </c>
+      <c r="BQ32">
+        <f t="shared" si="11"/>
+        <v>30.783930466106554</v>
+      </c>
+      <c r="BR32">
+        <f t="shared" si="11"/>
+        <v>30.682677629927788</v>
+      </c>
+      <c r="BS32">
+        <f t="shared" si="11"/>
+        <v>30.581757829091782</v>
+      </c>
+      <c r="BT32">
+        <f t="shared" si="11"/>
+        <v>30.481169968196731</v>
+      </c>
+      <c r="BU32">
+        <f t="shared" si="11"/>
+        <v>30.380912955443765</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <f>SUM(B32:BU32)</f>
+        <v>2464.5899999999992</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35">
+        <f>2000*(1+A13)^(72)</f>
+        <v>2535.4116258407485</v>
+      </c>
+      <c r="C35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36">
+        <f>5000-B35</f>
         <v>2464.5883741592515</v>
       </c>
     </row>

</xml_diff>